<commit_message>
Updated substitution table to add "unitless"
Updated substitution table to add "unitless"  and some other fixes
</commit_message>
<xml_diff>
--- a/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
+++ b/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Box Sync\EMLUnits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9BA728-738D-4E32-9BD4-57A9D167918E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B128FC-BD1D-4347-81CC-D48F015F98B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="480" windowWidth="18960" windowHeight="14340" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
+    <workbookView xWindow="-21210" yWindow="375" windowWidth="18960" windowHeight="14340" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="630">
   <si>
     <t>singular</t>
   </si>
@@ -1793,13 +1793,184 @@
     <t>umolm-2s-1</t>
   </si>
   <si>
-    <t>MicroMol-PER-M2-SEC</t>
-  </si>
-  <si>
     <t>shoots</t>
   </si>
   <si>
     <t>shoot</t>
+  </si>
+  <si>
+    <t>nanomol</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>BYTE</t>
+  </si>
+  <si>
+    <t>-s$</t>
+  </si>
+  <si>
+    <t>get rid of trailing -s</t>
+  </si>
+  <si>
+    <t>BFT</t>
+  </si>
+  <si>
+    <t>beaufort</t>
+  </si>
+  <si>
+    <t>becquerel</t>
+  </si>
+  <si>
+    <t>BQ</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>coulomb</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>centimenter</t>
+  </si>
+  <si>
+    <t>centi-</t>
+  </si>
+  <si>
+    <t>Centi</t>
+  </si>
+  <si>
+    <t>centi--</t>
+  </si>
+  <si>
+    <t>^mg$</t>
+  </si>
+  <si>
+    <t>fathom</t>
+  </si>
+  <si>
+    <t>FATH</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>-carbon</t>
+  </si>
+  <si>
+    <t>_Carbon-</t>
+  </si>
+  <si>
+    <t>^ms$</t>
+  </si>
+  <si>
+    <t>MilliSEC</t>
+  </si>
+  <si>
+    <t>HectoPA</t>
+  </si>
+  <si>
+    <t>Misspelled pseudounit</t>
+  </si>
+  <si>
+    <t>horsepower</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>kilogrampercubitmeter</t>
+  </si>
+  <si>
+    <t>KiloGM-PER-M3</t>
+  </si>
+  <si>
+    <t>metre</t>
+  </si>
+  <si>
+    <t>squaremeterpersquaresecond</t>
+  </si>
+  <si>
+    <t>M2-PER-SEC2</t>
+  </si>
+  <si>
+    <t>giga-</t>
+  </si>
+  <si>
+    <t>Giga</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>UNITLESS</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>dimmessionless</t>
+  </si>
+  <si>
+    <t>nounits</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>^n$</t>
+  </si>
+  <si>
+    <t>MOL-e-</t>
+  </si>
+  <si>
+    <t>MOL-</t>
+  </si>
+  <si>
+    <t>squaremillimeter</t>
+  </si>
+  <si>
+    <t>^kpa$</t>
+  </si>
+  <si>
+    <t>abundance</t>
+  </si>
+  <si>
+    <t>^um$</t>
+  </si>
+  <si>
+    <t>^hpa$</t>
+  </si>
+  <si>
+    <t>reciprocalday</t>
+  </si>
+  <si>
+    <t>PER-DAY</t>
+  </si>
+  <si>
+    <t>mols-</t>
+  </si>
+  <si>
+    <t>W-PER-M2</t>
+  </si>
+  <si>
+    <t>^wm-2$</t>
+  </si>
+  <si>
+    <t>MOL--e-</t>
+  </si>
+  <si>
+    <t>footus</t>
   </si>
 </sst>
 </file>
@@ -2191,11 +2362,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843A9CED-DCDD-4961-A3EA-063485F1C458}">
-  <dimension ref="A1:D269"/>
+  <dimension ref="A1:D311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C256" sqref="C256:C259"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,68 +2426,69 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>456</v>
+        <v>618</v>
       </c>
       <c r="B5" t="s">
-        <v>457</v>
+        <v>357</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="B6" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>453</v>
+        <v>480</v>
       </c>
       <c r="B7" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7"/>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>500</v>
+        <v>453</v>
       </c>
       <c r="B8" t="s">
-        <v>501</v>
+        <v>454</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>500</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>501</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2324,10 +2496,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>506</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
-        <v>507</v>
+        <v>211</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2335,7 +2507,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B12" t="s">
         <v>507</v>
@@ -2346,10 +2518,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>507</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2357,7 +2529,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="B14" t="s">
         <v>196</v>
@@ -2368,10 +2540,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="B15" t="s">
-        <v>514</v>
+        <v>196</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2379,10 +2551,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>543</v>
+        <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>544</v>
+        <v>514</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2390,21 +2562,18 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>545</v>
+        <v>623</v>
       </c>
       <c r="B17" t="s">
-        <v>546</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>624</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>569</v>
+        <v>543</v>
       </c>
       <c r="B18" t="s">
-        <v>570</v>
+        <v>544</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2412,68 +2581,65 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>545</v>
       </c>
       <c r="B19" t="s">
-        <v>529</v>
+        <v>546</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>531</v>
+        <v>569</v>
       </c>
       <c r="B20" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>442</v>
+        <v>572</v>
       </c>
       <c r="B21" t="s">
-        <v>443</v>
+        <v>492</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>603</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>604</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>516</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="B24" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2481,10 +2647,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>485</v>
+        <v>442</v>
       </c>
       <c r="B25" t="s">
-        <v>486</v>
+        <v>443</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2492,10 +2658,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>513</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>514</v>
+        <v>257</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2503,24 +2669,24 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>471</v>
+        <v>516</v>
       </c>
       <c r="B27" t="s">
-        <v>472</v>
+        <v>517</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>473</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>277</v>
+        <v>521</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>522</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2528,10 +2694,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>485</v>
       </c>
       <c r="B29" t="s">
-        <v>242</v>
+        <v>486</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2539,10 +2705,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>279</v>
+        <v>513</v>
       </c>
       <c r="B30" t="s">
-        <v>269</v>
+        <v>514</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2550,21 +2716,24 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>493</v>
+        <v>471</v>
       </c>
       <c r="B31" t="s">
-        <v>268</v>
+        <v>472</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
+      <c r="D31" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>277</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2572,10 +2741,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>455</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2583,10 +2752,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>494</v>
+        <v>279</v>
       </c>
       <c r="B34" t="s">
-        <v>495</v>
+        <v>269</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2594,24 +2763,21 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>526</v>
+        <v>493</v>
       </c>
       <c r="B35" t="s">
-        <v>527</v>
+        <v>268</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>496</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>497</v>
+        <v>268</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2619,24 +2785,21 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B37" t="s">
-        <v>460</v>
+        <v>268</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>467</v>
+        <v>494</v>
       </c>
       <c r="B38" t="s">
-        <v>342</v>
+        <v>495</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2644,21 +2807,24 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>464</v>
+        <v>526</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>527</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
+      <c r="D39" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="B40" t="s">
-        <v>273</v>
+        <v>497</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2666,21 +2832,24 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="B41" t="s">
-        <v>273</v>
+        <v>460</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
+      <c r="D41" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>426</v>
+        <v>467</v>
       </c>
       <c r="B42" t="s">
-        <v>427</v>
+        <v>342</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -2688,10 +2857,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>419</v>
+        <v>464</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>234</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -2699,10 +2868,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>420</v>
+        <v>448</v>
       </c>
       <c r="B44" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -2710,10 +2879,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>417</v>
+        <v>449</v>
       </c>
       <c r="B45" t="s">
-        <v>418</v>
+        <v>273</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -2721,10 +2890,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="B46" t="s">
-        <v>408</v>
+        <v>427</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -2732,236 +2901,230 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>390</v>
+        <v>419</v>
       </c>
       <c r="B47" t="s">
-        <v>391</v>
+        <v>308</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>420</v>
+      </c>
+      <c r="B48" t="s">
+        <v>308</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>417</v>
+      </c>
+      <c r="B49" t="s">
+        <v>418</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>407</v>
+      </c>
+      <c r="B50" t="s">
+        <v>408</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>390</v>
+      </c>
+      <c r="B51" t="s">
+        <v>391</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>446</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>447</v>
       </c>
-      <c r="C48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>465</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>466</v>
       </c>
-      <c r="C49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>30</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B54" t="s">
         <v>253</v>
       </c>
-      <c r="C50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>484</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B55" t="s">
         <v>483</v>
       </c>
-      <c r="C51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>441</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B56" t="s">
         <v>483</v>
       </c>
-      <c r="C52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>411</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>412</v>
       </c>
-      <c r="C53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>31</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>238</v>
       </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>274</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>237</v>
       </c>
-      <c r="C55">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="C59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>311</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B60" t="s">
         <v>213</v>
       </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="C60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>399</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>339</v>
       </c>
-      <c r="C57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="C61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>363</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B62" t="s">
         <v>339</v>
       </c>
-      <c r="C58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>17</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B63" t="s">
         <v>340</v>
       </c>
-      <c r="C59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="C63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>35</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B64" t="s">
         <v>254</v>
       </c>
-      <c r="C60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>395</v>
-      </c>
-      <c r="B61" t="s">
-        <v>396</v>
-      </c>
-      <c r="C61">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>509</v>
-      </c>
-      <c r="B62" t="s">
-        <v>282</v>
-      </c>
-      <c r="C62">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>286</v>
-      </c>
-      <c r="B63" t="s">
-        <v>282</v>
-      </c>
-      <c r="C63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>434</v>
-      </c>
-      <c r="B64" t="s">
-        <v>282</v>
-      </c>
       <c r="C64">
         <v>3</v>
-      </c>
-      <c r="D64" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>560</v>
+        <v>395</v>
       </c>
       <c r="B65" t="s">
-        <v>282</v>
+        <v>396</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>461</v>
+        <v>509</v>
       </c>
       <c r="B66" t="s">
         <v>282</v>
       </c>
       <c r="C66">
-        <v>4</v>
-      </c>
-      <c r="D66" t="s">
-        <v>292</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B67" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -2969,43 +3132,49 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>505</v>
+        <v>434</v>
       </c>
       <c r="B68" t="s">
-        <v>504</v>
+        <v>282</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
       <c r="B69" t="s">
-        <v>504</v>
+        <v>282</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>518</v>
+        <v>461</v>
       </c>
       <c r="B70" t="s">
-        <v>519</v>
+        <v>282</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>287</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -3013,21 +3182,21 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>558</v>
+        <v>505</v>
       </c>
       <c r="B72" t="s">
-        <v>443</v>
+        <v>504</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>503</v>
       </c>
       <c r="B73" t="s">
-        <v>258</v>
+        <v>504</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -3035,10 +3204,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>444</v>
+        <v>518</v>
       </c>
       <c r="B74" t="s">
-        <v>314</v>
+        <v>519</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -3046,10 +3215,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>314</v>
+        <v>251</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -3057,10 +3226,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>422</v>
+        <v>558</v>
       </c>
       <c r="B76" t="s">
-        <v>423</v>
+        <v>443</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -3068,24 +3237,21 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>468</v>
+        <v>39</v>
       </c>
       <c r="B77" t="s">
-        <v>469</v>
+        <v>258</v>
       </c>
       <c r="C77">
         <v>3</v>
-      </c>
-      <c r="D77" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>424</v>
+        <v>510</v>
       </c>
       <c r="B78" t="s">
-        <v>425</v>
+        <v>596</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -3093,21 +3259,24 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>512</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>596</v>
       </c>
       <c r="C79">
         <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>34</v>
+        <v>444</v>
       </c>
       <c r="B80" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -3115,10 +3284,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>36</v>
+        <v>313</v>
       </c>
       <c r="B81" t="s">
-        <v>212</v>
+        <v>314</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -3126,21 +3295,24 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>374</v>
+        <v>600</v>
       </c>
       <c r="B82" t="s">
-        <v>212</v>
+        <v>601</v>
       </c>
       <c r="C82">
         <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>40</v>
+        <v>422</v>
       </c>
       <c r="B83" t="s">
-        <v>260</v>
+        <v>423</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -3148,21 +3320,24 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>405</v>
+        <v>468</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>469</v>
       </c>
       <c r="C84">
         <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>424</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>425</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -3170,10 +3345,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>368</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>369</v>
+        <v>213</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -3181,10 +3356,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B87" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -3192,10 +3367,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>487</v>
+        <v>36</v>
       </c>
       <c r="B88" t="s">
-        <v>265</v>
+        <v>212</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -3203,45 +3378,43 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>374</v>
       </c>
       <c r="B89" t="s">
-        <v>265</v>
+        <v>212</v>
       </c>
       <c r="C89">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>474</v>
+        <v>40</v>
       </c>
       <c r="B90" t="s">
-        <v>475</v>
+        <v>260</v>
       </c>
       <c r="C90">
         <v>3</v>
       </c>
-      <c r="D90"/>
-    </row>
-    <row r="91" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>502</v>
+        <v>405</v>
       </c>
       <c r="B91" t="s">
-        <v>475</v>
+        <v>260</v>
       </c>
       <c r="C91">
-        <v>4</v>
-      </c>
-      <c r="D91"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>445</v>
+        <v>59</v>
       </c>
       <c r="B92" t="s">
-        <v>334</v>
+        <v>261</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -3249,10 +3422,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>333</v>
+        <v>368</v>
       </c>
       <c r="B93" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="C93">
         <v>3</v>
@@ -3260,24 +3433,21 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>409</v>
+        <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>334</v>
+        <v>262</v>
       </c>
       <c r="C94">
         <v>3</v>
-      </c>
-      <c r="D94" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>413</v>
+        <v>487</v>
       </c>
       <c r="B95" t="s">
-        <v>349</v>
+        <v>265</v>
       </c>
       <c r="C95">
         <v>3</v>
@@ -3285,46 +3455,45 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>348</v>
+        <v>50</v>
       </c>
       <c r="B96" t="s">
-        <v>349</v>
+        <v>265</v>
       </c>
       <c r="C96">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B97" t="s">
-        <v>262</v>
+        <v>475</v>
       </c>
       <c r="C97">
         <v>3</v>
       </c>
-      <c r="D97" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97"/>
+    </row>
+    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>379</v>
+        <v>502</v>
       </c>
       <c r="B98" t="s">
-        <v>262</v>
+        <v>475</v>
       </c>
       <c r="C98">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D98"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>445</v>
       </c>
       <c r="B99" t="s">
-        <v>476</v>
+        <v>334</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -3332,10 +3501,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>399</v>
+        <v>333</v>
       </c>
       <c r="B100" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C100">
         <v>3</v>
@@ -3343,21 +3512,24 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>20</v>
+        <v>409</v>
       </c>
       <c r="B101" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C101">
         <v>3</v>
+      </c>
+      <c r="D101" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>294</v>
+        <v>413</v>
       </c>
       <c r="B102" t="s">
-        <v>295</v>
+        <v>349</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -3365,10 +3537,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>348</v>
       </c>
       <c r="B103" t="s">
-        <v>264</v>
+        <v>349</v>
       </c>
       <c r="C103">
         <v>3</v>
@@ -3376,24 +3548,24 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>421</v>
+        <v>478</v>
       </c>
       <c r="B104" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C104">
         <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>292</v>
+        <v>479</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>379</v>
       </c>
       <c r="B105" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -3401,10 +3573,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B106" t="s">
-        <v>265</v>
+        <v>476</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -3412,10 +3584,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>491</v>
+        <v>399</v>
       </c>
       <c r="B107" t="s">
-        <v>492</v>
+        <v>339</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -3423,10 +3595,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>452</v>
+        <v>339</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -3434,10 +3606,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="B109" t="s">
-        <v>337</v>
+        <v>295</v>
       </c>
       <c r="C109">
         <v>3</v>
@@ -3445,211 +3617,214 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>512</v>
+        <v>14</v>
       </c>
       <c r="B110" t="s">
-        <v>511</v>
+        <v>264</v>
       </c>
       <c r="C110">
         <v>3</v>
-      </c>
-      <c r="D110" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>510</v>
+        <v>421</v>
       </c>
       <c r="B111" t="s">
-        <v>511</v>
+        <v>244</v>
       </c>
       <c r="C111">
         <v>3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>244</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" t="s">
+        <v>265</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>491</v>
+      </c>
+      <c r="B114" t="s">
+        <v>492</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>451</v>
+      </c>
+      <c r="B115" t="s">
+        <v>452</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>336</v>
+      </c>
+      <c r="B116" t="s">
+        <v>337</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>512</v>
+      </c>
+      <c r="B117" t="s">
+        <v>511</v>
+      </c>
+      <c r="C117">
+        <v>3</v>
+      </c>
+      <c r="D117" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>510</v>
+      </c>
+      <c r="B118" t="s">
+        <v>511</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>598</v>
+      </c>
+      <c r="B119" t="s">
+        <v>599</v>
+      </c>
+      <c r="C119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>47</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B120" t="s">
         <v>267</v>
       </c>
-      <c r="C112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="C120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>49</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B121" t="s">
         <v>268</v>
       </c>
-      <c r="C113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="C121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>46</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B122" t="s">
         <v>477</v>
       </c>
-      <c r="C114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="C122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>536</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B123" t="s">
         <v>268</v>
       </c>
-      <c r="C115">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="C123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>537</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B124" t="s">
         <v>268</v>
       </c>
-      <c r="C116">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="C124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>57</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B125" t="s">
         <v>201</v>
       </c>
-      <c r="C117">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="C125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>56</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B126" t="s">
         <v>332</v>
       </c>
-      <c r="C118">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="C126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>276</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B127" t="s">
         <v>200</v>
       </c>
-      <c r="C119">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="C127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>51</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B128" t="s">
         <v>239</v>
-      </c>
-      <c r="C120">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>277</v>
-      </c>
-      <c r="B121" t="s">
-        <v>241</v>
-      </c>
-      <c r="C121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>53</v>
-      </c>
-      <c r="B122" t="s">
-        <v>240</v>
-      </c>
-      <c r="C122">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>55</v>
-      </c>
-      <c r="B123" t="s">
-        <v>196</v>
-      </c>
-      <c r="C123">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>48</v>
-      </c>
-      <c r="B124" t="s">
-        <v>199</v>
-      </c>
-      <c r="C124">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>278</v>
-      </c>
-      <c r="B125" t="s">
-        <v>198</v>
-      </c>
-      <c r="C125">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>54</v>
-      </c>
-      <c r="B126" t="s">
-        <v>252</v>
-      </c>
-      <c r="C126">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>280</v>
-      </c>
-      <c r="B127" t="s">
-        <v>281</v>
-      </c>
-      <c r="C127">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>439</v>
-      </c>
-      <c r="B128" t="s">
-        <v>440</v>
       </c>
       <c r="C128">
         <v>3</v>
@@ -3657,10 +3832,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>482</v>
+        <v>277</v>
       </c>
       <c r="B129" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="C129">
         <v>3</v>
@@ -3668,10 +3843,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>306</v>
+        <v>53</v>
       </c>
       <c r="B130" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C130">
         <v>3</v>
@@ -3679,10 +3854,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>312</v>
+        <v>55</v>
       </c>
       <c r="B131" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C131">
         <v>3</v>
@@ -3690,195 +3865,192 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>310</v>
+        <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="C132">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>353</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="C133">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>410</v>
+        <v>54</v>
       </c>
       <c r="B134" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="C134">
-        <v>4</v>
-      </c>
-      <c r="D134" t="s">
-        <v>292</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>26</v>
+        <v>280</v>
       </c>
       <c r="B135" t="s">
-        <v>226</v>
+        <v>281</v>
       </c>
       <c r="C135">
-        <v>4</v>
-      </c>
-      <c r="D135" t="s">
-        <v>292</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>335</v>
+        <v>439</v>
       </c>
       <c r="B136" t="s">
-        <v>327</v>
+        <v>440</v>
       </c>
       <c r="C136">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>326</v>
+        <v>482</v>
       </c>
       <c r="B137" t="s">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="C137">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="B138" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C138">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>23</v>
+        <v>312</v>
       </c>
       <c r="B139" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C139">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>30</v>
+        <v>310</v>
       </c>
       <c r="B140" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="C140">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>38</v>
+        <v>353</v>
       </c>
       <c r="B141" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C141">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="B142" t="s">
-        <v>430</v>
+        <v>226</v>
       </c>
       <c r="C142">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D142" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>438</v>
+        <v>26</v>
       </c>
       <c r="B143" t="s">
-        <v>432</v>
+        <v>226</v>
       </c>
       <c r="C143">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="B144" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C144">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>3</v>
+        <v>326</v>
       </c>
       <c r="B145" t="s">
-        <v>282</v>
+        <v>327</v>
       </c>
       <c r="C145">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>392</v>
+        <v>321</v>
       </c>
       <c r="B146" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="C146">
-        <v>5</v>
-      </c>
-      <c r="D146" t="s">
-        <v>292</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B147" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C147">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>403</v>
+        <v>30</v>
       </c>
       <c r="B148" t="s">
-        <v>404</v>
+        <v>253</v>
       </c>
       <c r="C148">
         <v>5</v>
@@ -3886,10 +4058,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B149" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -3897,10 +4069,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>6</v>
+        <v>429</v>
       </c>
       <c r="B150" t="s">
-        <v>214</v>
+        <v>430</v>
       </c>
       <c r="C150">
         <v>5</v>
@@ -3908,24 +4080,21 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="B151" t="s">
-        <v>214</v>
+        <v>432</v>
       </c>
       <c r="C151">
         <v>5</v>
       </c>
-      <c r="D151" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>559</v>
+        <v>350</v>
       </c>
       <c r="B152" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="C152">
         <v>5</v>
@@ -3933,10 +4102,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>515</v>
+        <v>578</v>
       </c>
       <c r="B153" t="s">
-        <v>378</v>
+        <v>577</v>
       </c>
       <c r="C153">
         <v>5</v>
@@ -3944,32 +4113,32 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>377</v>
+        <v>579</v>
       </c>
       <c r="B154" t="s">
-        <v>378</v>
+        <v>580</v>
       </c>
       <c r="C154">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C155" s="4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>581</v>
+      </c>
+      <c r="B155" t="s">
+        <v>574</v>
+      </c>
+      <c r="C155">
         <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>547</v>
+        <v>573</v>
       </c>
       <c r="B156" t="s">
-        <v>256</v>
+        <v>574</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -3977,10 +4146,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B157" t="s">
-        <v>546</v>
+        <v>282</v>
       </c>
       <c r="C157">
         <v>5</v>
@@ -3988,21 +4157,24 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>29</v>
+        <v>392</v>
       </c>
       <c r="B158" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C158">
         <v>5</v>
       </c>
+      <c r="D158" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B159" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="C159">
         <v>5</v>
@@ -4010,365 +4182,365 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>403</v>
       </c>
       <c r="B160" t="s">
-        <v>327</v>
+        <v>404</v>
       </c>
       <c r="C160">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>16</v>
+        <v>582</v>
       </c>
       <c r="B161" t="s">
-        <v>250</v>
+        <v>583</v>
       </c>
       <c r="C161">
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B162" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="C162">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>338</v>
+        <v>6</v>
       </c>
       <c r="B163" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C163">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>428</v>
       </c>
       <c r="B164" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="C164">
         <v>5</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>21</v>
+        <v>559</v>
       </c>
       <c r="B165" t="s">
-        <v>222</v>
+        <v>378</v>
       </c>
       <c r="C165">
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>385</v>
+        <v>515</v>
       </c>
       <c r="B166" t="s">
-        <v>217</v>
+        <v>378</v>
       </c>
       <c r="C166">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>25</v>
+        <v>377</v>
       </c>
       <c r="B167" t="s">
-        <v>259</v>
+        <v>378</v>
       </c>
       <c r="C167">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>288</v>
       </c>
       <c r="B168" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="C168">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>361</v>
+        <v>589</v>
       </c>
       <c r="B169" t="s">
-        <v>362</v>
+        <v>590</v>
       </c>
       <c r="C169">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>4</v>
+        <v>547</v>
       </c>
       <c r="B170" t="s">
-        <v>94</v>
+        <v>256</v>
       </c>
       <c r="C170">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B171" t="s">
-        <v>263</v>
+        <v>546</v>
       </c>
       <c r="C171">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>12</v>
+        <v>629</v>
       </c>
       <c r="B172" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C172">
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>489</v>
+        <v>591</v>
       </c>
       <c r="B173" t="s">
-        <v>220</v>
+        <v>527</v>
       </c>
       <c r="C173">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B174" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="C174">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>341</v>
+        <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>342</v>
+        <v>235</v>
       </c>
       <c r="C175">
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B176" t="s">
-        <v>218</v>
+        <v>327</v>
       </c>
       <c r="C176">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B177" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="C177">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>352</v>
+        <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C178">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>18</v>
+        <v>338</v>
       </c>
       <c r="B179" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C179">
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>328</v>
+        <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>329</v>
+        <v>236</v>
       </c>
       <c r="C180">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B181" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C181">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="B182" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C182">
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>414</v>
+        <v>25</v>
       </c>
       <c r="B183" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="C183">
         <v>5</v>
       </c>
-      <c r="D183" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B184" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C184">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>42</v>
+        <v>361</v>
       </c>
       <c r="B185" t="s">
-        <v>270</v>
+        <v>362</v>
       </c>
       <c r="C185">
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>323</v>
+        <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>324</v>
+        <v>94</v>
       </c>
       <c r="C186">
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>393</v>
+        <v>602</v>
       </c>
       <c r="B187" t="s">
-        <v>394</v>
+        <v>94</v>
       </c>
       <c r="C187">
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B188" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="C188">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>353</v>
+        <v>12</v>
       </c>
       <c r="B189" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="C189">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>24</v>
+        <v>489</v>
       </c>
       <c r="B190" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="C190">
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B191" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C191">
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c r="B192" t="s">
-        <v>223</v>
+        <v>342</v>
       </c>
       <c r="C192">
         <v>5</v>
@@ -4376,10 +4548,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>498</v>
+        <v>330</v>
       </c>
       <c r="B193" t="s">
-        <v>499</v>
+        <v>218</v>
       </c>
       <c r="C193">
         <v>5</v>
@@ -4387,211 +4559,211 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B194" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C194">
         <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B195">
-        <v>3</v>
+      <c r="A195" t="s">
+        <v>352</v>
+      </c>
+      <c r="B195" t="s">
+        <v>225</v>
       </c>
       <c r="C195">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>318</v>
+        <v>18</v>
       </c>
       <c r="B196" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="C196">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="B197" t="s">
-        <v>213</v>
+        <v>329</v>
       </c>
       <c r="C197">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="B198" t="s">
-        <v>358</v>
+        <v>234</v>
       </c>
       <c r="C198">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>290</v>
+        <v>375</v>
       </c>
       <c r="B199" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C199">
-        <v>6</v>
-      </c>
-      <c r="D199" t="s">
-        <v>293</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="B200" t="s">
-        <v>436</v>
+        <v>234</v>
       </c>
       <c r="C200">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D200" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>437</v>
+        <v>2</v>
       </c>
       <c r="B201" t="s">
-        <v>436</v>
+        <v>234</v>
       </c>
       <c r="C201">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>373</v>
+        <v>42</v>
       </c>
       <c r="B202" t="s">
-        <v>372</v>
+        <v>270</v>
       </c>
       <c r="C202">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>371</v>
+        <v>323</v>
       </c>
       <c r="B203" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="C203">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>304</v>
+        <v>393</v>
       </c>
       <c r="B204" t="s">
-        <v>297</v>
+        <v>394</v>
       </c>
       <c r="C204">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>296</v>
+        <v>11</v>
       </c>
       <c r="B205" t="s">
-        <v>297</v>
+        <v>246</v>
       </c>
       <c r="C205">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>298</v>
+        <v>353</v>
       </c>
       <c r="B206" t="s">
-        <v>299</v>
+        <v>226</v>
       </c>
       <c r="C206">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>389</v>
+        <v>24</v>
       </c>
       <c r="B207" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="C207">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>300</v>
+        <v>9</v>
       </c>
       <c r="B208" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="C208">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="B209" t="s">
-        <v>345</v>
+        <v>223</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>388</v>
+        <v>498</v>
       </c>
       <c r="B210" t="s">
-        <v>345</v>
+        <v>499</v>
       </c>
       <c r="C210">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>387</v>
+        <v>27</v>
       </c>
       <c r="B211" t="s">
-        <v>345</v>
+        <v>273</v>
       </c>
       <c r="C211">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>303</v>
-      </c>
-      <c r="B212" t="s">
-        <v>302</v>
+      <c r="A212" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B212">
+        <v>3</v>
       </c>
       <c r="C212">
         <v>6</v>
@@ -4599,10 +4771,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>386</v>
+        <v>318</v>
       </c>
       <c r="B213" t="s">
-        <v>302</v>
+        <v>238</v>
       </c>
       <c r="C213">
         <v>6</v>
@@ -4610,10 +4782,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="B214" t="s">
-        <v>302</v>
+        <v>213</v>
       </c>
       <c r="C214">
         <v>6</v>
@@ -4621,49 +4793,49 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>523</v>
+        <v>320</v>
       </c>
       <c r="B215" t="s">
-        <v>302</v>
+        <v>358</v>
       </c>
       <c r="C215">
         <v>6</v>
       </c>
-      <c r="D215" t="s">
-        <v>524</v>
-      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>525</v>
+        <v>290</v>
       </c>
       <c r="B216" t="s">
-        <v>302</v>
+        <v>214</v>
       </c>
       <c r="C216">
         <v>6</v>
       </c>
       <c r="D216" t="s">
-        <v>524</v>
+        <v>293</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>346</v>
+        <v>584</v>
       </c>
       <c r="B217" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="C217">
         <v>6</v>
       </c>
+      <c r="D217" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>370</v>
+        <v>587</v>
       </c>
       <c r="B218" t="s">
-        <v>347</v>
+        <v>586</v>
       </c>
       <c r="C218">
         <v>6</v>
@@ -4671,60 +4843,51 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>283</v>
+        <v>585</v>
       </c>
       <c r="B219" t="s">
-        <v>202</v>
+        <v>586</v>
       </c>
       <c r="C219">
         <v>6</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B220">
-        <v>2</v>
+      <c r="A220" t="s">
+        <v>435</v>
+      </c>
+      <c r="B220" t="s">
+        <v>436</v>
       </c>
       <c r="C220">
         <v>6</v>
       </c>
-      <c r="D220" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B221">
-        <v>2</v>
+      <c r="A221" t="s">
+        <v>437</v>
+      </c>
+      <c r="B221" t="s">
+        <v>436</v>
       </c>
       <c r="C221">
         <v>6</v>
       </c>
-      <c r="D221" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>317</v>
+        <v>605</v>
       </c>
       <c r="B222" t="s">
-        <v>237</v>
-      </c>
-      <c r="C222">
-        <v>6</v>
+        <v>606</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>316</v>
+        <v>373</v>
       </c>
       <c r="B223" t="s">
-        <v>212</v>
+        <v>372</v>
       </c>
       <c r="C223">
         <v>6</v>
@@ -4732,517 +4895,995 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>319</v>
+        <v>371</v>
       </c>
       <c r="B224" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="C224">
         <v>6</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D224" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="B225" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="C225">
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="B226" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C226">
         <v>6</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>343</v>
+        <v>298</v>
       </c>
       <c r="B227" t="s">
-        <v>236</v>
+        <v>299</v>
       </c>
       <c r="C227">
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B228" t="s">
-        <v>214</v>
+        <v>299</v>
       </c>
       <c r="C228">
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>354</v>
+        <v>300</v>
       </c>
       <c r="B229" t="s">
-        <v>214</v>
+        <v>299</v>
       </c>
       <c r="C229">
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B230" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C230">
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="B231" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C231">
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="B232" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C232">
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>364</v>
+        <v>303</v>
       </c>
       <c r="B233" t="s">
-        <v>365</v>
+        <v>302</v>
       </c>
       <c r="C233">
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B234" t="s">
-        <v>357</v>
+        <v>302</v>
       </c>
       <c r="C234">
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>366</v>
+        <v>301</v>
       </c>
       <c r="B235" t="s">
-        <v>367</v>
+        <v>302</v>
       </c>
       <c r="C235">
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>555</v>
+        <v>523</v>
       </c>
       <c r="B236" t="s">
-        <v>556</v>
+        <v>302</v>
       </c>
       <c r="C236">
         <v>6</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D236" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>376</v>
+        <v>525</v>
       </c>
       <c r="B237" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
       <c r="C237">
         <v>6</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D237" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="B238" t="s">
-        <v>308</v>
+        <v>347</v>
       </c>
       <c r="C238">
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1</v>
+        <v>370</v>
       </c>
       <c r="B239" t="s">
-        <v>266</v>
+        <v>347</v>
       </c>
       <c r="C239">
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>382</v>
+        <v>283</v>
       </c>
       <c r="B240" t="s">
-        <v>322</v>
+        <v>202</v>
       </c>
       <c r="C240">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>381</v>
-      </c>
-      <c r="B241" t="s">
-        <v>94</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B241">
+        <v>2</v>
       </c>
       <c r="C241">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>400</v>
-      </c>
-      <c r="B242" t="s">
-        <v>217</v>
+        <v>6</v>
+      </c>
+      <c r="D241" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
       </c>
       <c r="C242">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D242" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>401</v>
+        <v>317</v>
       </c>
       <c r="B243" t="s">
-        <v>349</v>
+        <v>237</v>
       </c>
       <c r="C243">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>384</v>
+        <v>316</v>
       </c>
       <c r="B244" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C244">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
       <c r="B245" t="s">
-        <v>235</v>
+        <v>357</v>
       </c>
       <c r="C245">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>406</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>325</v>
+      </c>
+      <c r="B246" t="s">
+        <v>282</v>
       </c>
       <c r="C246">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>415</v>
+        <v>331</v>
       </c>
       <c r="B247" t="s">
-        <v>416</v>
+        <v>266</v>
       </c>
       <c r="C247">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="B248" t="s">
-        <v>432</v>
+        <v>236</v>
       </c>
       <c r="C248">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>433</v>
+        <v>397</v>
       </c>
       <c r="B249" t="s">
-        <v>432</v>
+        <v>214</v>
       </c>
       <c r="C249">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>462</v>
+        <v>354</v>
       </c>
       <c r="B250" t="s">
-        <v>463</v>
+        <v>214</v>
       </c>
       <c r="C250">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>488</v>
+        <v>355</v>
       </c>
       <c r="B251" t="s">
-        <v>220</v>
+        <v>356</v>
       </c>
       <c r="C251">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>530</v>
+        <v>359</v>
       </c>
       <c r="B252" t="s">
-        <v>266</v>
+        <v>360</v>
       </c>
       <c r="C252">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>538</v>
+        <v>363</v>
       </c>
       <c r="B253" t="s">
-        <v>266</v>
+        <v>339</v>
       </c>
       <c r="C253">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>539</v>
+        <v>364</v>
       </c>
       <c r="B254" t="s">
-        <v>266</v>
+        <v>365</v>
       </c>
       <c r="C254">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>540</v>
+        <v>402</v>
       </c>
       <c r="B255" t="s">
-        <v>266</v>
+        <v>357</v>
       </c>
       <c r="C255">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>542</v>
+        <v>366</v>
       </c>
       <c r="B256" t="s">
-        <v>266</v>
+        <v>367</v>
       </c>
       <c r="C256">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="B257" t="s">
-        <v>266</v>
+        <v>556</v>
       </c>
       <c r="C257">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>571</v>
+        <v>625</v>
       </c>
       <c r="B258" t="s">
-        <v>266</v>
+        <v>617</v>
       </c>
       <c r="C258">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>572</v>
+        <v>376</v>
       </c>
       <c r="B259" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="C259">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>557</v>
+        <v>380</v>
       </c>
       <c r="B260" t="s">
-        <v>251</v>
+        <v>308</v>
       </c>
       <c r="C260">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>541</v>
+        <v>1</v>
       </c>
       <c r="B261" t="s">
         <v>266</v>
       </c>
       <c r="C261">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>588</v>
+      </c>
+      <c r="B262" t="s">
+        <v>295</v>
+      </c>
+      <c r="C262">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>594</v>
+      </c>
+      <c r="B263" t="s">
+        <v>595</v>
+      </c>
+      <c r="C263">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>382</v>
+      </c>
+      <c r="B264" t="s">
+        <v>322</v>
+      </c>
+      <c r="C264">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>381</v>
+      </c>
+      <c r="B265" t="s">
+        <v>94</v>
+      </c>
+      <c r="C265">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>400</v>
+      </c>
+      <c r="B266" t="s">
+        <v>217</v>
+      </c>
+      <c r="C266">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>401</v>
+      </c>
+      <c r="B267" t="s">
+        <v>349</v>
+      </c>
+      <c r="C267">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>619</v>
+      </c>
+      <c r="B268" t="s">
+        <v>314</v>
+      </c>
+      <c r="C268">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>384</v>
+      </c>
+      <c r="B269" t="s">
+        <v>216</v>
+      </c>
+      <c r="C269">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>627</v>
+      </c>
+      <c r="B270" t="s">
+        <v>626</v>
+      </c>
+      <c r="C270">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>383</v>
+      </c>
+      <c r="B271" t="s">
+        <v>235</v>
+      </c>
+      <c r="C271">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C272">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>415</v>
+      </c>
+      <c r="B273" t="s">
+        <v>416</v>
+      </c>
+      <c r="C273">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>431</v>
+      </c>
+      <c r="B274" t="s">
+        <v>432</v>
+      </c>
+      <c r="C274">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>433</v>
+      </c>
+      <c r="B275" t="s">
+        <v>432</v>
+      </c>
+      <c r="C275">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>462</v>
+      </c>
+      <c r="B276" t="s">
+        <v>463</v>
+      </c>
+      <c r="C276">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>488</v>
+      </c>
+      <c r="B277" t="s">
+        <v>220</v>
+      </c>
+      <c r="C277">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>530</v>
+      </c>
+      <c r="B278" t="s">
+        <v>266</v>
+      </c>
+      <c r="C278">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>538</v>
+      </c>
+      <c r="B279" t="s">
+        <v>266</v>
+      </c>
+      <c r="C279">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>539</v>
+      </c>
+      <c r="B280" t="s">
+        <v>266</v>
+      </c>
+      <c r="C280">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>540</v>
+      </c>
+      <c r="B281" t="s">
+        <v>266</v>
+      </c>
+      <c r="C281">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>542</v>
+      </c>
+      <c r="B282" t="s">
+        <v>266</v>
+      </c>
+      <c r="C282">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>562</v>
+      </c>
+      <c r="B283" t="s">
+        <v>266</v>
+      </c>
+      <c r="C283">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>570</v>
+      </c>
+      <c r="B284" t="s">
+        <v>266</v>
+      </c>
+      <c r="C284">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>571</v>
+      </c>
+      <c r="B285" t="s">
+        <v>266</v>
+      </c>
+      <c r="C285">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>620</v>
+      </c>
+      <c r="B286" t="s">
+        <v>266</v>
+      </c>
+      <c r="C286">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>557</v>
+      </c>
+      <c r="B287" t="s">
+        <v>251</v>
+      </c>
+      <c r="C287">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>541</v>
+      </c>
+      <c r="B288" t="s">
+        <v>266</v>
+      </c>
+      <c r="C288">
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
         <v>551</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B289" t="s">
         <v>266</v>
       </c>
-      <c r="C262">
+      <c r="C289">
         <v>8</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>616</v>
+      </c>
+      <c r="B290" t="s">
+        <v>617</v>
+      </c>
+      <c r="C290">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>628</v>
+      </c>
+      <c r="B291" t="s">
+        <v>617</v>
+      </c>
+      <c r="C291">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>622</v>
+      </c>
+      <c r="B292" t="s">
+        <v>596</v>
+      </c>
+      <c r="C292">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
         <v>490</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B293" t="s">
         <v>220</v>
       </c>
-      <c r="C263">
+      <c r="C293">
         <v>8</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="3" t="s">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>615</v>
+      </c>
+      <c r="B294" t="s">
+        <v>266</v>
+      </c>
+      <c r="C294">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>621</v>
+      </c>
+      <c r="B295" t="s">
+        <v>369</v>
+      </c>
+      <c r="C295">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>552</v>
+      </c>
+      <c r="B296" t="s">
+        <v>553</v>
+      </c>
+      <c r="C296">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>563</v>
+      </c>
+      <c r="B297" t="s">
+        <v>378</v>
+      </c>
+      <c r="C297">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>564</v>
+      </c>
+      <c r="B298" t="s">
+        <v>565</v>
+      </c>
+      <c r="C298">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>566</v>
+      </c>
+      <c r="B299" t="s">
+        <v>334</v>
+      </c>
+      <c r="C299">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="B300" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="C300">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B301" t="s">
+        <v>593</v>
+      </c>
+      <c r="C301">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>607</v>
+      </c>
+      <c r="B302" t="s">
+        <v>608</v>
+      </c>
+      <c r="C302">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>612</v>
+      </c>
+      <c r="B303" t="s">
+        <v>608</v>
+      </c>
+      <c r="C303">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>609</v>
+      </c>
+      <c r="B304" t="s">
+        <v>608</v>
+      </c>
+      <c r="C304">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>610</v>
+      </c>
+      <c r="B305" t="s">
+        <v>608</v>
+      </c>
+      <c r="C305">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>611</v>
+      </c>
+      <c r="B306" t="s">
+        <v>608</v>
+      </c>
+      <c r="C306">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>613</v>
+      </c>
+      <c r="B307" t="s">
+        <v>608</v>
+      </c>
+      <c r="C307">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>614</v>
+      </c>
+      <c r="B308" t="s">
+        <v>608</v>
+      </c>
+      <c r="C308">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>613</v>
+      </c>
+      <c r="B309" t="s">
+        <v>608</v>
+      </c>
+      <c r="C309">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="B264" s="3" t="s">
+      <c r="B310" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="C264">
+      <c r="C310">
         <v>8</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D310" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>552</v>
-      </c>
-      <c r="B265" t="s">
-        <v>553</v>
-      </c>
-      <c r="C265">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B311" s="3"/>
+      <c r="C311">
         <v>8</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>563</v>
-      </c>
-      <c r="B266" t="s">
-        <v>378</v>
-      </c>
-      <c r="C266">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>564</v>
-      </c>
-      <c r="B267" t="s">
-        <v>565</v>
-      </c>
-      <c r="C267">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>566</v>
-      </c>
-      <c r="B268" t="s">
-        <v>334</v>
-      </c>
-      <c r="C268">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="C269">
-        <v>8</v>
+      <c r="D311" t="s">
+        <v>576</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D224">
-    <sortCondition ref="C9:C224"/>
-    <sortCondition ref="A9:A224"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D245">
+    <sortCondition ref="C10:C245"/>
+    <sortCondition ref="A10:A245"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A few more tweaks added to the list
</commit_message>
<xml_diff>
--- a/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
+++ b/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Box Sync\EMLUnits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B128FC-BD1D-4347-81CC-D48F015F98B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72594FE0-91F1-4B75-92C0-7D949AA095A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21210" yWindow="375" windowWidth="18960" windowHeight="14340" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="651">
   <si>
     <t>singular</t>
   </si>
@@ -1916,9 +1916,6 @@
     <t>unitless</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>dimmessionless</t>
   </si>
   <si>
@@ -1971,6 +1968,72 @@
   </si>
   <si>
     <t>footus</t>
+  </si>
+  <si>
+    <t>BAN</t>
+  </si>
+  <si>
+    <t>^bans$</t>
+  </si>
+  <si>
+    <t>Centi-</t>
+  </si>
+  <si>
+    <t>chains</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>decigram</t>
+  </si>
+  <si>
+    <t>DeciGM</t>
+  </si>
+  <si>
+    <t>^na$</t>
+  </si>
+  <si>
+    <t>Centi--</t>
+  </si>
+  <si>
+    <t>microsiemens</t>
+  </si>
+  <si>
+    <t>^psu$</t>
+  </si>
+  <si>
+    <t>^ntu$</t>
+  </si>
+  <si>
+    <t>-NA$</t>
+  </si>
+  <si>
+    <t>get rid of trailing -NA</t>
+  </si>
+  <si>
+    <t>Deci--</t>
+  </si>
+  <si>
+    <t>giga--</t>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>mm3</t>
+  </si>
+  <si>
+    <t>litre</t>
+  </si>
+  <si>
+    <t>PER-CentiM2</t>
+  </si>
+  <si>
+    <t>percentimetercubed</t>
+  </si>
+  <si>
+    <t>PER-CentiM3</t>
   </si>
 </sst>
 </file>
@@ -2362,11 +2425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843A9CED-DCDD-4961-A3EA-063485F1C458}">
-  <dimension ref="A1:D311"/>
+  <dimension ref="A1:D331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,7 +2489,7 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B5" t="s">
         <v>357</v>
@@ -2483,23 +2546,24 @@
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>634</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>635</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2507,10 +2571,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>506</v>
+        <v>275</v>
       </c>
       <c r="B12" t="s">
-        <v>507</v>
+        <v>211</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2518,7 +2582,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B13" t="s">
         <v>507</v>
@@ -2529,10 +2593,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>507</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2540,7 +2604,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="B15" t="s">
         <v>196</v>
@@ -2551,10 +2615,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="B16" t="s">
-        <v>514</v>
+        <v>196</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2562,29 +2626,29 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>623</v>
+        <v>513</v>
       </c>
       <c r="B17" t="s">
-        <v>624</v>
+        <v>514</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>543</v>
+        <v>622</v>
       </c>
       <c r="B18" t="s">
-        <v>544</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+        <v>623</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B19" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2592,10 +2656,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>569</v>
+        <v>545</v>
       </c>
       <c r="B20" t="s">
-        <v>517</v>
+        <v>546</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2603,10 +2667,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B21" t="s">
-        <v>492</v>
+        <v>517</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2614,10 +2678,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>603</v>
+        <v>572</v>
       </c>
       <c r="B22" t="s">
-        <v>604</v>
+        <v>492</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2625,21 +2689,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>603</v>
       </c>
       <c r="B23" t="s">
-        <v>529</v>
+        <v>604</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>531</v>
+        <v>276</v>
       </c>
       <c r="B24" t="s">
-        <v>532</v>
+        <v>648</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2647,10 +2711,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>649</v>
       </c>
       <c r="B25" t="s">
-        <v>443</v>
+        <v>650</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2658,10 +2722,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>257</v>
+        <v>529</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2669,24 +2733,21 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>516</v>
+        <v>531</v>
       </c>
       <c r="B27" t="s">
-        <v>517</v>
+        <v>532</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>521</v>
+        <v>442</v>
       </c>
       <c r="B28" t="s">
-        <v>522</v>
+        <v>443</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2694,10 +2755,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>485</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>486</v>
+        <v>257</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2705,35 +2766,35 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="B30" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
+      <c r="D30" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>471</v>
+        <v>521</v>
       </c>
       <c r="B31" t="s">
-        <v>472</v>
+        <v>522</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>277</v>
+        <v>485</v>
       </c>
       <c r="B32" t="s">
-        <v>241</v>
+        <v>486</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2741,10 +2802,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>513</v>
       </c>
       <c r="B33" t="s">
-        <v>242</v>
+        <v>514</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2752,21 +2813,24 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>279</v>
+        <v>471</v>
       </c>
       <c r="B34" t="s">
-        <v>269</v>
+        <v>472</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
+      <c r="D34" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>493</v>
+        <v>277</v>
       </c>
       <c r="B35" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2774,10 +2838,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2785,10 +2849,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>455</v>
+        <v>279</v>
       </c>
       <c r="B37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2796,10 +2860,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B38" t="s">
-        <v>495</v>
+        <v>268</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2807,24 +2871,21 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>526</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>527</v>
+        <v>268</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>496</v>
+        <v>455</v>
       </c>
       <c r="B40" t="s">
-        <v>497</v>
+        <v>268</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2832,35 +2893,35 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>459</v>
+        <v>494</v>
       </c>
       <c r="B41" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>467</v>
+        <v>526</v>
       </c>
       <c r="B42" t="s">
-        <v>342</v>
+        <v>527</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
+      <c r="D42" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>464</v>
+        <v>496</v>
       </c>
       <c r="B43" t="s">
-        <v>234</v>
+        <v>497</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -2868,21 +2929,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="B44" t="s">
-        <v>273</v>
+        <v>460</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
+      <c r="D44" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>342</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -2890,10 +2954,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>426</v>
+        <v>464</v>
       </c>
       <c r="B46" t="s">
-        <v>427</v>
+        <v>234</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -2901,10 +2965,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="B47" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2912,10 +2976,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>420</v>
+        <v>449</v>
       </c>
       <c r="B48" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -2923,10 +2987,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B49" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -2934,10 +2998,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="B50" t="s">
-        <v>408</v>
+        <v>308</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -2945,43 +3009,43 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="B51" t="s">
-        <v>391</v>
+        <v>308</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>446</v>
+        <v>417</v>
       </c>
       <c r="B52" t="s">
-        <v>447</v>
+        <v>418</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>465</v>
+        <v>407</v>
       </c>
       <c r="B53" t="s">
-        <v>466</v>
+        <v>408</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>390</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>391</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -2989,10 +3053,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>484</v>
+        <v>446</v>
       </c>
       <c r="B55" t="s">
-        <v>483</v>
+        <v>447</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -3000,10 +3064,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>441</v>
+        <v>646</v>
       </c>
       <c r="B56" t="s">
-        <v>483</v>
+        <v>358</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -3011,10 +3075,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>411</v>
+        <v>465</v>
       </c>
       <c r="B57" t="s">
-        <v>412</v>
+        <v>466</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -3022,10 +3086,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -3033,10 +3097,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>274</v>
+        <v>484</v>
       </c>
       <c r="B59" t="s">
-        <v>237</v>
+        <v>483</v>
       </c>
       <c r="C59">
         <v>3</v>
@@ -3044,10 +3108,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>311</v>
+        <v>441</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>483</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -3055,10 +3119,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="B61" t="s">
-        <v>339</v>
+        <v>412</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -3066,10 +3130,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>363</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>339</v>
+        <v>238</v>
       </c>
       <c r="C62">
         <v>3</v>
@@ -3077,10 +3141,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>17</v>
+        <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>340</v>
+        <v>237</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -3088,10 +3152,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>311</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>213</v>
       </c>
       <c r="C64">
         <v>3</v>
@@ -3099,10 +3163,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B65" t="s">
-        <v>396</v>
+        <v>339</v>
       </c>
       <c r="C65">
         <v>3</v>
@@ -3110,10 +3174,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>509</v>
+        <v>363</v>
       </c>
       <c r="B66" t="s">
-        <v>282</v>
+        <v>339</v>
       </c>
       <c r="C66">
         <v>3</v>
@@ -3121,10 +3185,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>286</v>
+        <v>632</v>
       </c>
       <c r="B67" t="s">
-        <v>282</v>
+        <v>633</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -3132,49 +3196,43 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>434</v>
+        <v>195</v>
       </c>
       <c r="B68" t="s">
-        <v>282</v>
+        <v>633</v>
       </c>
       <c r="C68">
         <v>3</v>
-      </c>
-      <c r="D68" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>560</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>282</v>
+        <v>340</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>461</v>
+        <v>35</v>
       </c>
       <c r="B70" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="C70">
-        <v>4</v>
-      </c>
-      <c r="D70" t="s">
-        <v>292</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>289</v>
+        <v>395</v>
       </c>
       <c r="B71" t="s">
-        <v>287</v>
+        <v>396</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -3182,21 +3240,21 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B72" t="s">
-        <v>504</v>
+        <v>282</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>503</v>
+        <v>286</v>
       </c>
       <c r="B73" t="s">
-        <v>504</v>
+        <v>282</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -3204,43 +3262,49 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>518</v>
+        <v>434</v>
       </c>
       <c r="B74" t="s">
-        <v>519</v>
+        <v>282</v>
       </c>
       <c r="C74">
         <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>560</v>
       </c>
       <c r="B75" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>558</v>
+        <v>461</v>
       </c>
       <c r="B76" t="s">
-        <v>443</v>
+        <v>282</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="B77" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -3248,35 +3312,32 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="B78" t="s">
-        <v>596</v>
+        <v>504</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="B79" t="s">
-        <v>596</v>
+        <v>504</v>
       </c>
       <c r="C79">
         <v>3</v>
-      </c>
-      <c r="D79" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>444</v>
+        <v>518</v>
       </c>
       <c r="B80" t="s">
-        <v>314</v>
+        <v>519</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -3284,10 +3345,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>314</v>
+        <v>251</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -3295,24 +3356,21 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>600</v>
+        <v>558</v>
       </c>
       <c r="B82" t="s">
-        <v>601</v>
+        <v>443</v>
       </c>
       <c r="C82">
         <v>3</v>
-      </c>
-      <c r="D82" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>422</v>
+        <v>39</v>
       </c>
       <c r="B83" t="s">
-        <v>423</v>
+        <v>258</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -3320,35 +3378,35 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>468</v>
+        <v>510</v>
       </c>
       <c r="B84" t="s">
-        <v>469</v>
+        <v>596</v>
       </c>
       <c r="C84">
         <v>3</v>
-      </c>
-      <c r="D84" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>424</v>
+        <v>512</v>
       </c>
       <c r="B85" t="s">
-        <v>425</v>
+        <v>596</v>
       </c>
       <c r="C85">
         <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>444</v>
       </c>
       <c r="B86" t="s">
-        <v>213</v>
+        <v>314</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -3356,10 +3414,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>313</v>
       </c>
       <c r="B87" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -3367,21 +3425,24 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>36</v>
+        <v>600</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>601</v>
       </c>
       <c r="C88">
         <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>374</v>
+        <v>422</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>423</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -3389,21 +3450,24 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>468</v>
       </c>
       <c r="B90" t="s">
-        <v>260</v>
+        <v>469</v>
       </c>
       <c r="C90">
         <v>3</v>
+      </c>
+      <c r="D90" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>405</v>
+        <v>424</v>
       </c>
       <c r="B91" t="s">
-        <v>260</v>
+        <v>425</v>
       </c>
       <c r="C91">
         <v>3</v>
@@ -3411,10 +3475,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -3422,10 +3486,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>368</v>
+        <v>34</v>
       </c>
       <c r="B93" t="s">
-        <v>369</v>
+        <v>308</v>
       </c>
       <c r="C93">
         <v>3</v>
@@ -3433,10 +3497,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="C94">
         <v>3</v>
@@ -3444,10 +3508,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>487</v>
+        <v>374</v>
       </c>
       <c r="B95" t="s">
-        <v>265</v>
+        <v>212</v>
       </c>
       <c r="C95">
         <v>3</v>
@@ -3455,45 +3519,43 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B96" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C96">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>474</v>
+        <v>405</v>
       </c>
       <c r="B97" t="s">
-        <v>475</v>
+        <v>260</v>
       </c>
       <c r="C97">
         <v>3</v>
       </c>
-      <c r="D97"/>
-    </row>
-    <row r="98" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>502</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
-        <v>475</v>
+        <v>261</v>
       </c>
       <c r="C98">
-        <v>4</v>
-      </c>
-      <c r="D98"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>445</v>
+        <v>368</v>
       </c>
       <c r="B99" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -3501,10 +3563,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>333</v>
+        <v>28</v>
       </c>
       <c r="B100" t="s">
-        <v>334</v>
+        <v>262</v>
       </c>
       <c r="C100">
         <v>3</v>
@@ -3512,82 +3574,84 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>409</v>
+        <v>487</v>
       </c>
       <c r="B101" t="s">
-        <v>334</v>
+        <v>265</v>
       </c>
       <c r="C101">
         <v>3</v>
-      </c>
-      <c r="D101" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>413</v>
+        <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>349</v>
+        <v>265</v>
       </c>
       <c r="C102">
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>348</v>
+        <v>474</v>
       </c>
       <c r="B103" t="s">
-        <v>349</v>
+        <v>475</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103"/>
+    </row>
+    <row r="104" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>478</v>
+        <v>502</v>
       </c>
       <c r="B104" t="s">
-        <v>262</v>
+        <v>475</v>
       </c>
       <c r="C104">
-        <v>3</v>
-      </c>
-      <c r="D104" t="s">
-        <v>479</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D104"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>379</v>
+        <v>445</v>
       </c>
       <c r="B105" t="s">
-        <v>262</v>
+        <v>334</v>
       </c>
       <c r="C105">
         <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>43</v>
+        <v>333</v>
       </c>
       <c r="B106" t="s">
-        <v>476</v>
+        <v>334</v>
       </c>
       <c r="C106">
         <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="B107" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -3595,10 +3659,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>20</v>
+        <v>638</v>
       </c>
       <c r="B108" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -3606,10 +3670,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>294</v>
+        <v>409</v>
       </c>
       <c r="B109" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="C109">
         <v>3</v>
@@ -3617,10 +3681,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>409</v>
       </c>
       <c r="B110" t="s">
-        <v>264</v>
+        <v>334</v>
       </c>
       <c r="C110">
         <v>3</v>
@@ -3628,24 +3692,21 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B111" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="C111">
         <v>3</v>
-      </c>
-      <c r="D111" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>5</v>
+        <v>348</v>
       </c>
       <c r="B112" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="C112">
         <v>3</v>
@@ -3653,21 +3714,24 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>50</v>
+        <v>478</v>
       </c>
       <c r="B113" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C113">
         <v>3</v>
+      </c>
+      <c r="D113" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>491</v>
+        <v>379</v>
       </c>
       <c r="B114" t="s">
-        <v>492</v>
+        <v>262</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -3675,10 +3739,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>451</v>
+        <v>43</v>
       </c>
       <c r="B115" t="s">
-        <v>452</v>
+        <v>476</v>
       </c>
       <c r="C115">
         <v>3</v>
@@ -3686,10 +3750,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>336</v>
+        <v>399</v>
       </c>
       <c r="B116" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C116">
         <v>3</v>
@@ -3697,24 +3761,21 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
       <c r="B117" t="s">
-        <v>511</v>
+        <v>339</v>
       </c>
       <c r="C117">
         <v>3</v>
-      </c>
-      <c r="D117" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>510</v>
+        <v>294</v>
       </c>
       <c r="B118" t="s">
-        <v>511</v>
+        <v>295</v>
       </c>
       <c r="C118">
         <v>3</v>
@@ -3722,10 +3783,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>598</v>
+        <v>14</v>
       </c>
       <c r="B119" t="s">
-        <v>599</v>
+        <v>264</v>
       </c>
       <c r="C119">
         <v>3</v>
@@ -3733,21 +3794,24 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>47</v>
+        <v>421</v>
       </c>
       <c r="B120" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="C120">
         <v>3</v>
+      </c>
+      <c r="D120" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B121" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C121">
         <v>3</v>
@@ -3755,10 +3819,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B122" t="s">
-        <v>477</v>
+        <v>265</v>
       </c>
       <c r="C122">
         <v>3</v>
@@ -3766,10 +3830,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>536</v>
+        <v>491</v>
       </c>
       <c r="B123" t="s">
-        <v>268</v>
+        <v>492</v>
       </c>
       <c r="C123">
         <v>3</v>
@@ -3777,10 +3841,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>537</v>
+        <v>451</v>
       </c>
       <c r="B124" t="s">
-        <v>268</v>
+        <v>452</v>
       </c>
       <c r="C124">
         <v>3</v>
@@ -3788,10 +3852,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>57</v>
+        <v>336</v>
       </c>
       <c r="B125" t="s">
-        <v>201</v>
+        <v>337</v>
       </c>
       <c r="C125">
         <v>3</v>
@@ -3799,21 +3863,24 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>56</v>
+        <v>512</v>
       </c>
       <c r="B126" t="s">
-        <v>332</v>
+        <v>511</v>
       </c>
       <c r="C126">
         <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>276</v>
+        <v>510</v>
       </c>
       <c r="B127" t="s">
-        <v>200</v>
+        <v>511</v>
       </c>
       <c r="C127">
         <v>3</v>
@@ -3821,335 +3888,335 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>598</v>
+      </c>
+      <c r="B128" t="s">
+        <v>599</v>
+      </c>
+      <c r="C128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>47</v>
+      </c>
+      <c r="B129" t="s">
+        <v>267</v>
+      </c>
+      <c r="C129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>49</v>
+      </c>
+      <c r="B130" t="s">
+        <v>268</v>
+      </c>
+      <c r="C130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>46</v>
+      </c>
+      <c r="B131" t="s">
+        <v>477</v>
+      </c>
+      <c r="C131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>536</v>
+      </c>
+      <c r="B132" t="s">
+        <v>268</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>537</v>
+      </c>
+      <c r="B133" t="s">
+        <v>268</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>57</v>
+      </c>
+      <c r="B134" t="s">
+        <v>201</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>56</v>
+      </c>
+      <c r="B135" t="s">
+        <v>332</v>
+      </c>
+      <c r="C135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>276</v>
+      </c>
+      <c r="B136" t="s">
+        <v>200</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>51</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B137" t="s">
         <v>239</v>
       </c>
-      <c r="C128">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="C137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>277</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B138" t="s">
         <v>241</v>
       </c>
-      <c r="C129">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="C138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>53</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B139" t="s">
         <v>240</v>
       </c>
-      <c r="C130">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="C139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>55</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B140" t="s">
         <v>196</v>
       </c>
-      <c r="C131">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="C140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>48</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B141" t="s">
         <v>199</v>
       </c>
-      <c r="C132">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="C141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>278</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B142" t="s">
         <v>198</v>
       </c>
-      <c r="C133">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="C142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>54</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B143" t="s">
         <v>252</v>
       </c>
-      <c r="C134">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="C143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>280</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B144" t="s">
         <v>281</v>
       </c>
-      <c r="C135">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>439</v>
-      </c>
-      <c r="B136" t="s">
-        <v>440</v>
-      </c>
-      <c r="C136">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>482</v>
-      </c>
-      <c r="B137" t="s">
-        <v>196</v>
-      </c>
-      <c r="C137">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>306</v>
-      </c>
-      <c r="B138" t="s">
-        <v>237</v>
-      </c>
-      <c r="C138">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>312</v>
-      </c>
-      <c r="B139" t="s">
-        <v>212</v>
-      </c>
-      <c r="C139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>310</v>
-      </c>
-      <c r="B140" t="s">
-        <v>226</v>
-      </c>
-      <c r="C140">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>353</v>
-      </c>
-      <c r="B141" t="s">
-        <v>226</v>
-      </c>
-      <c r="C141">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>410</v>
-      </c>
-      <c r="B142" t="s">
-        <v>226</v>
-      </c>
-      <c r="C142">
-        <v>4</v>
-      </c>
-      <c r="D142" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>26</v>
-      </c>
-      <c r="B143" t="s">
-        <v>226</v>
-      </c>
-      <c r="C143">
-        <v>4</v>
-      </c>
-      <c r="D143" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>335</v>
-      </c>
-      <c r="B144" t="s">
-        <v>327</v>
-      </c>
       <c r="C144">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>326</v>
+        <v>439</v>
       </c>
       <c r="B145" t="s">
-        <v>327</v>
+        <v>440</v>
       </c>
       <c r="C145">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>321</v>
+        <v>482</v>
       </c>
       <c r="B146" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="C146">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>23</v>
+        <v>306</v>
       </c>
       <c r="B147" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="C147">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>30</v>
+        <v>312</v>
       </c>
       <c r="B148" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="C148">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>38</v>
+        <v>310</v>
       </c>
       <c r="B149" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C149">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>429</v>
+        <v>353</v>
       </c>
       <c r="B150" t="s">
-        <v>430</v>
+        <v>226</v>
       </c>
       <c r="C150">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>438</v>
+        <v>410</v>
       </c>
       <c r="B151" t="s">
-        <v>432</v>
+        <v>226</v>
       </c>
       <c r="C151">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D151" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>350</v>
+        <v>26</v>
       </c>
       <c r="B152" t="s">
-        <v>351</v>
+        <v>226</v>
       </c>
       <c r="C152">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D152" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>578</v>
+        <v>335</v>
       </c>
       <c r="B153" t="s">
-        <v>577</v>
+        <v>327</v>
       </c>
       <c r="C153">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>579</v>
+        <v>326</v>
       </c>
       <c r="B154" t="s">
-        <v>580</v>
+        <v>327</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>581</v>
+        <v>321</v>
       </c>
       <c r="B155" t="s">
-        <v>574</v>
+        <v>223</v>
       </c>
       <c r="C155">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>573</v>
+        <v>23</v>
       </c>
       <c r="B156" t="s">
-        <v>574</v>
+        <v>272</v>
       </c>
       <c r="C156">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B157" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="C157">
         <v>5</v>
@@ -4157,24 +4224,21 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>392</v>
+        <v>38</v>
       </c>
       <c r="B158" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="C158">
         <v>5</v>
       </c>
-      <c r="D158" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>7</v>
+        <v>429</v>
       </c>
       <c r="B159" t="s">
-        <v>245</v>
+        <v>430</v>
       </c>
       <c r="C159">
         <v>5</v>
@@ -4182,10 +4246,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>403</v>
+        <v>438</v>
       </c>
       <c r="B160" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
       <c r="C160">
         <v>5</v>
@@ -4193,10 +4257,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>582</v>
+        <v>350</v>
       </c>
       <c r="B161" t="s">
-        <v>583</v>
+        <v>351</v>
       </c>
       <c r="C161">
         <v>5</v>
@@ -4204,10 +4268,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>578</v>
       </c>
       <c r="B162" t="s">
-        <v>248</v>
+        <v>577</v>
       </c>
       <c r="C162">
         <v>5</v>
@@ -4215,10 +4279,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>6</v>
+        <v>579</v>
       </c>
       <c r="B163" t="s">
-        <v>214</v>
+        <v>580</v>
       </c>
       <c r="C163">
         <v>5</v>
@@ -4226,24 +4290,21 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>428</v>
+        <v>581</v>
       </c>
       <c r="B164" t="s">
-        <v>214</v>
+        <v>574</v>
       </c>
       <c r="C164">
         <v>5</v>
       </c>
-      <c r="D164" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>559</v>
+        <v>573</v>
       </c>
       <c r="B165" t="s">
-        <v>378</v>
+        <v>574</v>
       </c>
       <c r="C165">
         <v>5</v>
@@ -4251,10 +4312,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>515</v>
+        <v>3</v>
       </c>
       <c r="B166" t="s">
-        <v>378</v>
+        <v>282</v>
       </c>
       <c r="C166">
         <v>5</v>
@@ -4262,32 +4323,35 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>377</v>
+        <v>392</v>
       </c>
       <c r="B167" t="s">
-        <v>378</v>
+        <v>245</v>
       </c>
       <c r="C167">
         <v>5</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>288</v>
+        <v>7</v>
       </c>
       <c r="B168" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="C168">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>589</v>
+        <v>403</v>
       </c>
       <c r="B169" t="s">
-        <v>590</v>
+        <v>404</v>
       </c>
       <c r="C169">
         <v>5</v>
@@ -4295,10 +4359,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>547</v>
+        <v>582</v>
       </c>
       <c r="B170" t="s">
-        <v>256</v>
+        <v>583</v>
       </c>
       <c r="C170">
         <v>5</v>
@@ -4306,10 +4370,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B171" t="s">
-        <v>546</v>
+        <v>248</v>
       </c>
       <c r="C171">
         <v>5</v>
@@ -4317,10 +4381,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>629</v>
+        <v>6</v>
       </c>
       <c r="B172" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
       <c r="C172">
         <v>5</v>
@@ -4328,21 +4392,24 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>591</v>
+        <v>428</v>
       </c>
       <c r="B173" t="s">
-        <v>527</v>
+        <v>214</v>
       </c>
       <c r="C173">
         <v>5</v>
       </c>
+      <c r="D173" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>29</v>
+        <v>559</v>
       </c>
       <c r="B174" t="s">
-        <v>255</v>
+        <v>378</v>
       </c>
       <c r="C174">
         <v>5</v>
@@ -4350,10 +4417,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>8</v>
+        <v>515</v>
       </c>
       <c r="B175" t="s">
-        <v>235</v>
+        <v>378</v>
       </c>
       <c r="C175">
         <v>5</v>
@@ -4361,32 +4428,32 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>326</v>
+        <v>377</v>
       </c>
       <c r="B176" t="s">
-        <v>327</v>
+        <v>378</v>
       </c>
       <c r="C176">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>16</v>
+        <v>288</v>
       </c>
       <c r="B177" t="s">
-        <v>250</v>
+        <v>287</v>
       </c>
       <c r="C177">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>33</v>
+        <v>589</v>
       </c>
       <c r="B178" t="s">
-        <v>215</v>
+        <v>590</v>
       </c>
       <c r="C178">
         <v>5</v>
@@ -4394,10 +4461,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>338</v>
+        <v>547</v>
       </c>
       <c r="B179" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="C179">
         <v>5</v>
@@ -4405,10 +4472,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B180" t="s">
-        <v>236</v>
+        <v>546</v>
       </c>
       <c r="C180">
         <v>5</v>
@@ -4416,10 +4483,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>21</v>
+        <v>628</v>
       </c>
       <c r="B181" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="C181">
         <v>5</v>
@@ -4427,10 +4494,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>385</v>
+        <v>591</v>
       </c>
       <c r="B182" t="s">
-        <v>217</v>
+        <v>527</v>
       </c>
       <c r="C182">
         <v>5</v>
@@ -4438,10 +4505,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B183" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C183">
         <v>5</v>
@@ -4449,10 +4516,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B184" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C184">
         <v>5</v>
@@ -4460,10 +4527,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
       <c r="B185" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
       <c r="C185">
         <v>5</v>
@@ -4471,10 +4538,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B186" t="s">
-        <v>94</v>
+        <v>250</v>
       </c>
       <c r="C186">
         <v>5</v>
@@ -4482,10 +4549,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>602</v>
+        <v>33</v>
       </c>
       <c r="B187" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
       <c r="C187">
         <v>5</v>
@@ -4493,10 +4560,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>32</v>
+        <v>338</v>
       </c>
       <c r="B188" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="C188">
         <v>5</v>
@@ -4504,10 +4571,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B189" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C189">
         <v>5</v>
@@ -4515,10 +4582,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>489</v>
+        <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C190">
         <v>5</v>
@@ -4526,10 +4593,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>37</v>
+        <v>385</v>
       </c>
       <c r="B191" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C191">
         <v>5</v>
@@ -4537,189 +4604,186 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>341</v>
+        <v>25</v>
       </c>
       <c r="B192" t="s">
-        <v>342</v>
+        <v>259</v>
       </c>
       <c r="C192">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>330</v>
+        <v>15</v>
       </c>
       <c r="B193" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="C193">
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>1</v>
+        <v>647</v>
       </c>
       <c r="B194" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="C194">
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B195" t="s">
-        <v>225</v>
+        <v>362</v>
       </c>
       <c r="C195">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B196" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
       <c r="C196">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>328</v>
+        <v>602</v>
       </c>
       <c r="B197" t="s">
-        <v>329</v>
+        <v>94</v>
       </c>
       <c r="C197">
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B198" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
       <c r="C198">
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>375</v>
+        <v>12</v>
       </c>
       <c r="B199" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="C199">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>414</v>
+        <v>489</v>
       </c>
       <c r="B200" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C200">
         <v>5</v>
       </c>
-      <c r="D200" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C201">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>42</v>
+        <v>341</v>
       </c>
       <c r="B202" t="s">
-        <v>270</v>
+        <v>342</v>
       </c>
       <c r="C202">
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B203" t="s">
-        <v>324</v>
+        <v>218</v>
       </c>
       <c r="C203">
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>393</v>
+        <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>394</v>
+        <v>266</v>
       </c>
       <c r="C204">
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>11</v>
+        <v>352</v>
       </c>
       <c r="B205" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="C205">
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>353</v>
+        <v>18</v>
       </c>
       <c r="B206" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C206">
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>24</v>
+        <v>328</v>
       </c>
       <c r="B207" t="s">
-        <v>271</v>
+        <v>329</v>
       </c>
       <c r="C207">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B208" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C208">
         <v>5</v>
@@ -4727,10 +4791,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>309</v>
+        <v>375</v>
       </c>
       <c r="B209" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="C209">
         <v>5</v>
@@ -4738,156 +4802,156 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>498</v>
+        <v>414</v>
       </c>
       <c r="B210" t="s">
-        <v>499</v>
+        <v>234</v>
       </c>
       <c r="C210">
         <v>5</v>
       </c>
+      <c r="D210" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B211" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="C211">
         <v>5</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="B212">
-        <v>3</v>
+      <c r="A212" t="s">
+        <v>42</v>
+      </c>
+      <c r="B212" t="s">
+        <v>270</v>
       </c>
       <c r="C212">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B213" t="s">
-        <v>238</v>
+        <v>324</v>
       </c>
       <c r="C213">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>315</v>
+        <v>393</v>
       </c>
       <c r="B214" t="s">
-        <v>213</v>
+        <v>394</v>
       </c>
       <c r="C214">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>320</v>
+        <v>11</v>
       </c>
       <c r="B215" t="s">
-        <v>358</v>
+        <v>246</v>
       </c>
       <c r="C215">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>290</v>
+        <v>353</v>
       </c>
       <c r="B216" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="C216">
-        <v>6</v>
-      </c>
-      <c r="D216" t="s">
-        <v>293</v>
+        <v>5</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>584</v>
+        <v>24</v>
       </c>
       <c r="B217" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="C217">
-        <v>6</v>
-      </c>
-      <c r="D217" t="s">
-        <v>292</v>
+        <v>5</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>587</v>
+        <v>9</v>
       </c>
       <c r="B218" t="s">
-        <v>586</v>
+        <v>224</v>
       </c>
       <c r="C218">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>585</v>
+        <v>309</v>
       </c>
       <c r="B219" t="s">
-        <v>586</v>
+        <v>223</v>
       </c>
       <c r="C219">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>435</v>
+        <v>498</v>
       </c>
       <c r="B220" t="s">
-        <v>436</v>
+        <v>499</v>
       </c>
       <c r="C220">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>437</v>
+        <v>27</v>
       </c>
       <c r="B221" t="s">
-        <v>436</v>
+        <v>273</v>
       </c>
       <c r="C221">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B222">
+        <v>3</v>
+      </c>
+      <c r="C222">
         <v>6</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>605</v>
-      </c>
-      <c r="B222" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>373</v>
+        <v>318</v>
       </c>
       <c r="B223" t="s">
-        <v>372</v>
+        <v>238</v>
       </c>
       <c r="C223">
         <v>6</v>
@@ -4895,24 +4959,21 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>371</v>
+        <v>315</v>
       </c>
       <c r="B224" t="s">
-        <v>372</v>
+        <v>213</v>
       </c>
       <c r="C224">
         <v>6</v>
       </c>
-      <c r="D224" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B225" t="s">
-        <v>297</v>
+        <v>358</v>
       </c>
       <c r="C225">
         <v>6</v>
@@ -4920,32 +4981,38 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B226" t="s">
-        <v>297</v>
+        <v>214</v>
       </c>
       <c r="C226">
         <v>6</v>
       </c>
+      <c r="D226" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>298</v>
+        <v>584</v>
       </c>
       <c r="B227" t="s">
-        <v>299</v>
+        <v>245</v>
       </c>
       <c r="C227">
         <v>6</v>
       </c>
+      <c r="D227" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>389</v>
+        <v>587</v>
       </c>
       <c r="B228" t="s">
-        <v>299</v>
+        <v>586</v>
       </c>
       <c r="C228">
         <v>6</v>
@@ -4953,10 +5020,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>300</v>
+        <v>585</v>
       </c>
       <c r="B229" t="s">
-        <v>299</v>
+        <v>586</v>
       </c>
       <c r="C229">
         <v>6</v>
@@ -4964,10 +5031,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>344</v>
+        <v>637</v>
       </c>
       <c r="B230" t="s">
-        <v>345</v>
+        <v>586</v>
       </c>
       <c r="C230">
         <v>6</v>
@@ -4975,10 +5042,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>388</v>
+        <v>631</v>
       </c>
       <c r="B231" t="s">
-        <v>345</v>
+        <v>586</v>
       </c>
       <c r="C231">
         <v>6</v>
@@ -4986,10 +5053,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>387</v>
+        <v>435</v>
       </c>
       <c r="B232" t="s">
-        <v>345</v>
+        <v>436</v>
       </c>
       <c r="C232">
         <v>6</v>
@@ -4997,10 +5064,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>303</v>
+        <v>437</v>
       </c>
       <c r="B233" t="s">
-        <v>302</v>
+        <v>436</v>
       </c>
       <c r="C233">
         <v>6</v>
@@ -5008,10 +5075,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>386</v>
+        <v>643</v>
       </c>
       <c r="B234" t="s">
-        <v>302</v>
+        <v>436</v>
       </c>
       <c r="C234">
         <v>6</v>
@@ -5019,10 +5086,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>301</v>
+        <v>643</v>
       </c>
       <c r="B235" t="s">
-        <v>302</v>
+        <v>436</v>
       </c>
       <c r="C235">
         <v>6</v>
@@ -5030,38 +5097,32 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>523</v>
+        <v>644</v>
       </c>
       <c r="B236" t="s">
-        <v>302</v>
+        <v>606</v>
       </c>
       <c r="C236">
         <v>6</v>
       </c>
-      <c r="D236" t="s">
-        <v>524</v>
-      </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>525</v>
+        <v>605</v>
       </c>
       <c r="B237" t="s">
-        <v>302</v>
+        <v>606</v>
       </c>
       <c r="C237">
         <v>6</v>
       </c>
-      <c r="D237" t="s">
-        <v>524</v>
-      </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>346</v>
+        <v>373</v>
       </c>
       <c r="B238" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="C238">
         <v>6</v>
@@ -5069,60 +5130,57 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B239" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="C239">
         <v>6</v>
       </c>
+      <c r="D239" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="B240" t="s">
-        <v>202</v>
+        <v>297</v>
       </c>
       <c r="C240">
         <v>6</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B241">
-        <v>2</v>
+      <c r="A241" t="s">
+        <v>296</v>
+      </c>
+      <c r="B241" t="s">
+        <v>297</v>
       </c>
       <c r="C241">
         <v>6</v>
       </c>
-      <c r="D241" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B242">
-        <v>2</v>
+      <c r="A242" t="s">
+        <v>298</v>
+      </c>
+      <c r="B242" t="s">
+        <v>299</v>
       </c>
       <c r="C242">
         <v>6</v>
       </c>
-      <c r="D242" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>317</v>
+        <v>389</v>
       </c>
       <c r="B243" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
       <c r="C243">
         <v>6</v>
@@ -5130,10 +5188,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B244" t="s">
-        <v>212</v>
+        <v>299</v>
       </c>
       <c r="C244">
         <v>6</v>
@@ -5141,10 +5199,10 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="B245" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="C245">
         <v>6</v>
@@ -5152,10 +5210,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>325</v>
+        <v>388</v>
       </c>
       <c r="B246" t="s">
-        <v>282</v>
+        <v>345</v>
       </c>
       <c r="C246">
         <v>6</v>
@@ -5163,10 +5221,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="B247" t="s">
-        <v>266</v>
+        <v>345</v>
       </c>
       <c r="C247">
         <v>6</v>
@@ -5174,10 +5232,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>343</v>
+        <v>303</v>
       </c>
       <c r="B248" t="s">
-        <v>236</v>
+        <v>302</v>
       </c>
       <c r="C248">
         <v>6</v>
@@ -5185,10 +5243,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="B249" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
       <c r="C249">
         <v>6</v>
@@ -5196,10 +5254,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>354</v>
+        <v>301</v>
       </c>
       <c r="B250" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
       <c r="C250">
         <v>6</v>
@@ -5207,32 +5265,38 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>355</v>
+        <v>523</v>
       </c>
       <c r="B251" t="s">
-        <v>356</v>
+        <v>302</v>
       </c>
       <c r="C251">
         <v>6</v>
       </c>
+      <c r="D251" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>359</v>
+        <v>525</v>
       </c>
       <c r="B252" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
       <c r="C252">
         <v>6</v>
       </c>
+      <c r="D252" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="B253" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="C253">
         <v>6</v>
@@ -5240,10 +5304,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="B254" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="C254">
         <v>6</v>
@@ -5251,252 +5315,258 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>402</v>
+        <v>283</v>
       </c>
       <c r="B255" t="s">
-        <v>357</v>
+        <v>202</v>
       </c>
       <c r="C255">
         <v>6</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>366</v>
-      </c>
-      <c r="B256" t="s">
-        <v>367</v>
+      <c r="A256" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
       </c>
       <c r="C256">
         <v>6</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>555</v>
-      </c>
-      <c r="B257" t="s">
-        <v>556</v>
+      <c r="D256" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B257">
+        <v>2</v>
       </c>
       <c r="C257">
         <v>6</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>625</v>
+        <v>317</v>
       </c>
       <c r="B258" t="s">
-        <v>617</v>
+        <v>237</v>
       </c>
       <c r="C258">
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>376</v>
+        <v>316</v>
       </c>
       <c r="B259" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C259">
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="B260" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="C260">
         <v>6</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="B261" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="C261">
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>588</v>
+        <v>331</v>
       </c>
       <c r="B262" t="s">
-        <v>295</v>
+        <v>266</v>
       </c>
       <c r="C262">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>594</v>
+        <v>343</v>
       </c>
       <c r="B263" t="s">
-        <v>595</v>
+        <v>236</v>
       </c>
       <c r="C263">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="B264" t="s">
-        <v>322</v>
+        <v>214</v>
       </c>
       <c r="C264">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="B265" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="C265">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>400</v>
+        <v>355</v>
       </c>
       <c r="B266" t="s">
-        <v>217</v>
+        <v>356</v>
       </c>
       <c r="C266">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>401</v>
+        <v>359</v>
       </c>
       <c r="B267" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="C267">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>619</v>
+        <v>363</v>
       </c>
       <c r="B268" t="s">
-        <v>314</v>
+        <v>339</v>
       </c>
       <c r="C268">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="B269" t="s">
-        <v>216</v>
+        <v>365</v>
       </c>
       <c r="C269">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>627</v>
+        <v>402</v>
       </c>
       <c r="B270" t="s">
-        <v>626</v>
+        <v>357</v>
       </c>
       <c r="C270">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="B271" t="s">
-        <v>235</v>
+        <v>367</v>
       </c>
       <c r="C271">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>406</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>555</v>
+      </c>
+      <c r="B272" t="s">
+        <v>556</v>
       </c>
       <c r="C272">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>415</v>
+        <v>624</v>
       </c>
       <c r="B273" t="s">
-        <v>416</v>
+        <v>616</v>
       </c>
       <c r="C273">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>431</v>
+        <v>376</v>
       </c>
       <c r="B274" t="s">
-        <v>432</v>
+        <v>214</v>
       </c>
       <c r="C274">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="B275" t="s">
-        <v>432</v>
+        <v>308</v>
       </c>
       <c r="C275">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>462</v>
+        <v>1</v>
       </c>
       <c r="B276" t="s">
-        <v>463</v>
+        <v>266</v>
       </c>
       <c r="C276">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>488</v>
+        <v>588</v>
       </c>
       <c r="B277" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="C277">
         <v>7</v>
@@ -5504,10 +5574,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>530</v>
+        <v>594</v>
       </c>
       <c r="B278" t="s">
-        <v>266</v>
+        <v>595</v>
       </c>
       <c r="C278">
         <v>7</v>
@@ -5515,10 +5585,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>538</v>
+        <v>382</v>
       </c>
       <c r="B279" t="s">
-        <v>266</v>
+        <v>322</v>
       </c>
       <c r="C279">
         <v>7</v>
@@ -5526,10 +5596,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>539</v>
+        <v>381</v>
       </c>
       <c r="B280" t="s">
-        <v>266</v>
+        <v>94</v>
       </c>
       <c r="C280">
         <v>7</v>
@@ -5537,10 +5607,10 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>540</v>
+        <v>400</v>
       </c>
       <c r="B281" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="C281">
         <v>7</v>
@@ -5548,10 +5618,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>542</v>
+        <v>401</v>
       </c>
       <c r="B282" t="s">
-        <v>266</v>
+        <v>349</v>
       </c>
       <c r="C282">
         <v>7</v>
@@ -5559,10 +5629,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>562</v>
+        <v>618</v>
       </c>
       <c r="B283" t="s">
-        <v>266</v>
+        <v>314</v>
       </c>
       <c r="C283">
         <v>7</v>
@@ -5570,10 +5640,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>570</v>
+        <v>384</v>
       </c>
       <c r="B284" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="C284">
         <v>7</v>
@@ -5581,10 +5651,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>571</v>
+        <v>626</v>
       </c>
       <c r="B285" t="s">
-        <v>266</v>
+        <v>625</v>
       </c>
       <c r="C285">
         <v>7</v>
@@ -5592,21 +5662,21 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>620</v>
+        <v>383</v>
       </c>
       <c r="B286" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="C286">
         <v>7</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>557</v>
-      </c>
-      <c r="B287" t="s">
-        <v>251</v>
+      <c r="A287" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>406</v>
       </c>
       <c r="C287">
         <v>7</v>
@@ -5614,276 +5684,496 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>541</v>
+        <v>415</v>
       </c>
       <c r="B288" t="s">
-        <v>266</v>
+        <v>416</v>
       </c>
       <c r="C288">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>551</v>
+        <v>431</v>
       </c>
       <c r="B289" t="s">
-        <v>266</v>
+        <v>432</v>
       </c>
       <c r="C289">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>616</v>
+        <v>433</v>
       </c>
       <c r="B290" t="s">
-        <v>617</v>
+        <v>432</v>
       </c>
       <c r="C290">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B291" t="s">
-        <v>617</v>
+        <v>629</v>
       </c>
       <c r="C291">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>622</v>
+        <v>462</v>
       </c>
       <c r="B292" t="s">
-        <v>596</v>
+        <v>463</v>
       </c>
       <c r="C292">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B293" t="s">
         <v>220</v>
       </c>
       <c r="C293">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>615</v>
+        <v>530</v>
       </c>
       <c r="B294" t="s">
         <v>266</v>
       </c>
       <c r="C294">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>621</v>
+        <v>538</v>
       </c>
       <c r="B295" t="s">
-        <v>369</v>
+        <v>266</v>
       </c>
       <c r="C295">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="B296" t="s">
-        <v>553</v>
+        <v>266</v>
       </c>
       <c r="C296">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>563</v>
+        <v>540</v>
       </c>
       <c r="B297" t="s">
-        <v>378</v>
+        <v>266</v>
       </c>
       <c r="C297">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>564</v>
+        <v>542</v>
       </c>
       <c r="B298" t="s">
-        <v>565</v>
+        <v>266</v>
       </c>
       <c r="C298">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B299" t="s">
-        <v>334</v>
+        <v>266</v>
       </c>
       <c r="C299">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="B300" s="3" t="s">
-        <v>568</v>
+      <c r="A300" t="s">
+        <v>570</v>
+      </c>
+      <c r="B300" t="s">
+        <v>266</v>
       </c>
       <c r="C300">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A301" s="3" t="s">
-        <v>592</v>
+      <c r="A301" t="s">
+        <v>571</v>
       </c>
       <c r="B301" t="s">
-        <v>593</v>
+        <v>266</v>
       </c>
       <c r="C301">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>607</v>
+        <v>619</v>
       </c>
       <c r="B302" t="s">
-        <v>608</v>
+        <v>266</v>
       </c>
       <c r="C302">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>612</v>
+        <v>645</v>
       </c>
       <c r="B303" t="s">
-        <v>608</v>
+        <v>266</v>
       </c>
       <c r="C303">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>609</v>
+        <v>557</v>
       </c>
       <c r="B304" t="s">
-        <v>608</v>
+        <v>251</v>
       </c>
       <c r="C304">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>610</v>
+        <v>541</v>
       </c>
       <c r="B305" t="s">
-        <v>608</v>
+        <v>266</v>
       </c>
       <c r="C305">
         <v>8</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>611</v>
+        <v>551</v>
       </c>
       <c r="B306" t="s">
-        <v>608</v>
+        <v>266</v>
       </c>
       <c r="C306">
         <v>8</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B307" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="C307">
         <v>8</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>614</v>
+        <v>627</v>
       </c>
       <c r="B308" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="C308">
         <v>8</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="B309" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="C309">
         <v>8</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="B310" s="3" t="s">
-        <v>549</v>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>490</v>
+      </c>
+      <c r="B310" t="s">
+        <v>220</v>
       </c>
       <c r="C310">
         <v>8</v>
       </c>
-      <c r="D310" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="B311" s="3"/>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>614</v>
+      </c>
+      <c r="B311" t="s">
+        <v>266</v>
+      </c>
       <c r="C311">
         <v>8</v>
       </c>
-      <c r="D311" t="s">
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>620</v>
+      </c>
+      <c r="B312" t="s">
+        <v>369</v>
+      </c>
+      <c r="C312">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>552</v>
+      </c>
+      <c r="B313" t="s">
+        <v>553</v>
+      </c>
+      <c r="C313">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>639</v>
+      </c>
+      <c r="B314" t="s">
+        <v>497</v>
+      </c>
+      <c r="C314">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>640</v>
+      </c>
+      <c r="B315" t="s">
+        <v>452</v>
+      </c>
+      <c r="C315">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>563</v>
+      </c>
+      <c r="B316" t="s">
+        <v>378</v>
+      </c>
+      <c r="C316">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>564</v>
+      </c>
+      <c r="B317" t="s">
+        <v>565</v>
+      </c>
+      <c r="C317">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>566</v>
+      </c>
+      <c r="B318" t="s">
+        <v>334</v>
+      </c>
+      <c r="C318">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="C319">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B320" t="s">
+        <v>593</v>
+      </c>
+      <c r="C320">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>607</v>
+      </c>
+      <c r="B321" t="s">
+        <v>608</v>
+      </c>
+      <c r="C321">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>611</v>
+      </c>
+      <c r="B322" t="s">
+        <v>608</v>
+      </c>
+      <c r="C322">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>609</v>
+      </c>
+      <c r="B323" t="s">
+        <v>608</v>
+      </c>
+      <c r="C323">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>610</v>
+      </c>
+      <c r="B324" t="s">
+        <v>608</v>
+      </c>
+      <c r="C324">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>636</v>
+      </c>
+      <c r="B325" t="s">
+        <v>608</v>
+      </c>
+      <c r="C325">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>612</v>
+      </c>
+      <c r="B326" t="s">
+        <v>608</v>
+      </c>
+      <c r="C326">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>613</v>
+      </c>
+      <c r="B327" t="s">
+        <v>608</v>
+      </c>
+      <c r="C327">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>612</v>
+      </c>
+      <c r="B328" t="s">
+        <v>608</v>
+      </c>
+      <c r="C328">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="C329">
+        <v>8</v>
+      </c>
+      <c r="D329" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B330" s="3"/>
+      <c r="C330">
+        <v>8</v>
+      </c>
+      <c r="D330" t="s">
         <v>576</v>
       </c>
     </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C331">
+        <v>8</v>
+      </c>
+      <c r="D331" t="s">
+        <v>642</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D245">
-    <sortCondition ref="C10:C245"/>
-    <sortCondition ref="A10:A245"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:D260">
+    <sortCondition ref="C11:C260"/>
+    <sortCondition ref="A11:A260"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated a few substitutions
Convert GigaGM to KiloTONNE and Killo to Kilo
</commit_message>
<xml_diff>
--- a/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
+++ b/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\EMLUnits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jhp7e\Box Sync\EMLUnits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD92875-99CB-4102-9E4F-A9A1B1EF06BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4578DA84-D3F9-407F-A7B0-8C37FD08D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="945" windowWidth="23190" windowHeight="12285" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
+    <workbookView xWindow="2895" yWindow="5625" windowWidth="21600" windowHeight="11295" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="745">
   <si>
     <t>singular</t>
   </si>
@@ -2301,6 +2301,21 @@
   </si>
   <si>
     <t>umoleco2</t>
+  </si>
+  <si>
+    <t>GigaGM</t>
+  </si>
+  <si>
+    <t>KiloTONNE</t>
+  </si>
+  <si>
+    <t>Giga-GM</t>
+  </si>
+  <si>
+    <t>Killo</t>
+  </si>
+  <si>
+    <t>killo</t>
   </si>
 </sst>
 </file>
@@ -2712,11 +2727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843A9CED-DCDD-4961-A3EA-063485F1C458}">
-  <dimension ref="A1:D396"/>
+  <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B305" sqref="B305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6116,10 +6131,10 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" t="s">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="B301" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C301">
         <v>6</v>
@@ -6127,18 +6142,15 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" t="s">
-        <v>387</v>
+        <v>744</v>
       </c>
       <c r="B302" t="s">
-        <v>298</v>
-      </c>
-      <c r="C302">
-        <v>6</v>
+        <v>296</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B303" t="s">
         <v>298</v>
@@ -6149,10 +6161,10 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" t="s">
-        <v>343</v>
+        <v>387</v>
       </c>
       <c r="B304" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="C304">
         <v>6</v>
@@ -6160,10 +6172,10 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" t="s">
-        <v>386</v>
+        <v>299</v>
       </c>
       <c r="B305" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="C305">
         <v>6</v>
@@ -6171,7 +6183,7 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="B306" t="s">
         <v>344</v>
@@ -6182,10 +6194,10 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" t="s">
-        <v>302</v>
+        <v>386</v>
       </c>
       <c r="B307" t="s">
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="C307">
         <v>6</v>
@@ -6193,10 +6205,10 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B308" t="s">
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="C308">
         <v>6</v>
@@ -6204,7 +6216,7 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B309" t="s">
         <v>301</v>
@@ -6215,7 +6227,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" t="s">
-        <v>518</v>
+        <v>384</v>
       </c>
       <c r="B310" t="s">
         <v>301</v>
@@ -6223,13 +6235,10 @@
       <c r="C310">
         <v>6</v>
       </c>
-      <c r="D310" t="s">
-        <v>519</v>
-      </c>
     </row>
     <row r="311" spans="1:4">
       <c r="A311" t="s">
-        <v>520</v>
+        <v>300</v>
       </c>
       <c r="B311" t="s">
         <v>301</v>
@@ -6237,38 +6246,41 @@
       <c r="C311">
         <v>6</v>
       </c>
-      <c r="D311" t="s">
-        <v>519</v>
-      </c>
     </row>
     <row r="312" spans="1:4">
       <c r="A312" t="s">
-        <v>345</v>
+        <v>518</v>
       </c>
       <c r="B312" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="C312">
         <v>6</v>
       </c>
+      <c r="D312" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="313" spans="1:4">
       <c r="A313" t="s">
-        <v>368</v>
+        <v>520</v>
       </c>
       <c r="B313" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="C313">
         <v>6</v>
       </c>
+      <c r="D313" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="314" spans="1:4">
       <c r="A314" t="s">
-        <v>647</v>
+        <v>345</v>
       </c>
       <c r="B314" t="s">
-        <v>648</v>
+        <v>346</v>
       </c>
       <c r="C314">
         <v>6</v>
@@ -6276,10 +6288,10 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" t="s">
-        <v>649</v>
+        <v>368</v>
       </c>
       <c r="B315" t="s">
-        <v>648</v>
+        <v>346</v>
       </c>
       <c r="C315">
         <v>6</v>
@@ -6287,71 +6299,71 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" t="s">
-        <v>282</v>
+        <v>647</v>
       </c>
       <c r="B316" t="s">
-        <v>202</v>
+        <v>648</v>
       </c>
       <c r="C316">
         <v>6</v>
       </c>
     </row>
     <row r="317" spans="1:4">
-      <c r="A317" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B317">
-        <v>2</v>
+      <c r="A317" t="s">
+        <v>649</v>
+      </c>
+      <c r="B317" t="s">
+        <v>648</v>
       </c>
       <c r="C317">
         <v>6</v>
       </c>
-      <c r="D317" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="318" spans="1:4">
-      <c r="A318" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B318">
-        <v>2</v>
+      <c r="A318" t="s">
+        <v>282</v>
+      </c>
+      <c r="B318" t="s">
+        <v>202</v>
       </c>
       <c r="C318">
         <v>6</v>
       </c>
-      <c r="D318" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="319" spans="1:4">
-      <c r="A319" t="s">
-        <v>316</v>
-      </c>
-      <c r="B319" t="s">
-        <v>237</v>
+      <c r="A319" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B319">
+        <v>2</v>
       </c>
       <c r="C319">
         <v>6</v>
       </c>
+      <c r="D319" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="320" spans="1:4">
-      <c r="A320" t="s">
-        <v>315</v>
-      </c>
-      <c r="B320" t="s">
-        <v>212</v>
+      <c r="A320" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B320">
+        <v>2</v>
       </c>
       <c r="C320">
         <v>6</v>
       </c>
+      <c r="D320" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B321" t="s">
-        <v>355</v>
+        <v>237</v>
       </c>
       <c r="C321">
         <v>6</v>
@@ -6359,10 +6371,10 @@
     </row>
     <row r="322" spans="1:3">
       <c r="A322" t="s">
-        <v>644</v>
+        <v>315</v>
       </c>
       <c r="B322" t="s">
-        <v>440</v>
+        <v>212</v>
       </c>
       <c r="C322">
         <v>6</v>
@@ -6370,10 +6382,10 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" t="s">
-        <v>645</v>
+        <v>318</v>
       </c>
       <c r="B323" t="s">
-        <v>646</v>
+        <v>355</v>
       </c>
       <c r="C323">
         <v>6</v>
@@ -6381,10 +6393,10 @@
     </row>
     <row r="324" spans="1:3">
       <c r="A324" t="s">
-        <v>324</v>
+        <v>644</v>
       </c>
       <c r="B324" t="s">
-        <v>281</v>
+        <v>440</v>
       </c>
       <c r="C324">
         <v>6</v>
@@ -6392,10 +6404,10 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
-        <v>330</v>
+        <v>645</v>
       </c>
       <c r="B325" t="s">
-        <v>265</v>
+        <v>646</v>
       </c>
       <c r="C325">
         <v>6</v>
@@ -6403,10 +6415,10 @@
     </row>
     <row r="326" spans="1:3">
       <c r="A326" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="C326">
         <v>6</v>
@@ -6414,10 +6426,10 @@
     </row>
     <row r="327" spans="1:3">
       <c r="A327" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="B327" t="s">
-        <v>354</v>
+        <v>265</v>
       </c>
       <c r="C327">
         <v>6</v>
@@ -6425,10 +6437,10 @@
     </row>
     <row r="328" spans="1:3">
       <c r="A328" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="B328" t="s">
-        <v>358</v>
+        <v>236</v>
       </c>
       <c r="C328">
         <v>6</v>
@@ -6436,10 +6448,10 @@
     </row>
     <row r="329" spans="1:3">
       <c r="A329" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="B329" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="C329">
         <v>6</v>
@@ -6447,10 +6459,10 @@
     </row>
     <row r="330" spans="1:3">
       <c r="A330" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B330" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C330">
         <v>6</v>
@@ -6458,10 +6470,10 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" t="s">
-        <v>399</v>
+        <v>361</v>
       </c>
       <c r="B331" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="C331">
         <v>6</v>
@@ -6469,10 +6481,10 @@
     </row>
     <row r="332" spans="1:3">
       <c r="A332" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B332" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C332">
         <v>6</v>
@@ -6480,10 +6492,10 @@
     </row>
     <row r="333" spans="1:3">
       <c r="A333" t="s">
-        <v>548</v>
+        <v>399</v>
       </c>
       <c r="B333" t="s">
-        <v>549</v>
+        <v>355</v>
       </c>
       <c r="C333">
         <v>6</v>
@@ -6491,10 +6503,10 @@
     </row>
     <row r="334" spans="1:3">
       <c r="A334" t="s">
-        <v>614</v>
+        <v>364</v>
       </c>
       <c r="B334" t="s">
-        <v>606</v>
+        <v>365</v>
       </c>
       <c r="C334">
         <v>6</v>
@@ -6502,10 +6514,10 @@
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>374</v>
+        <v>548</v>
       </c>
       <c r="B335" t="s">
-        <v>214</v>
+        <v>549</v>
       </c>
       <c r="C335">
         <v>6</v>
@@ -6513,10 +6525,10 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336" t="s">
-        <v>378</v>
+        <v>614</v>
       </c>
       <c r="B336" t="s">
-        <v>307</v>
+        <v>606</v>
       </c>
       <c r="C336">
         <v>6</v>
@@ -6524,10 +6536,10 @@
     </row>
     <row r="337" spans="1:3">
       <c r="A337" t="s">
-        <v>1</v>
+        <v>374</v>
       </c>
       <c r="B337" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="C337">
         <v>6</v>
@@ -6535,32 +6547,32 @@
     </row>
     <row r="338" spans="1:3">
       <c r="A338" t="s">
-        <v>580</v>
+        <v>378</v>
       </c>
       <c r="B338" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="C338">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="339" spans="1:3">
       <c r="A339" t="s">
-        <v>586</v>
+        <v>1</v>
       </c>
       <c r="B339" t="s">
-        <v>587</v>
+        <v>265</v>
       </c>
       <c r="C339">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="340" spans="1:3">
       <c r="A340" t="s">
-        <v>380</v>
+        <v>580</v>
       </c>
       <c r="B340" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="C340">
         <v>7</v>
@@ -6568,10 +6580,10 @@
     </row>
     <row r="341" spans="1:3">
       <c r="A341" t="s">
-        <v>379</v>
+        <v>586</v>
       </c>
       <c r="B341" t="s">
-        <v>94</v>
+        <v>587</v>
       </c>
       <c r="C341">
         <v>7</v>
@@ -6579,10 +6591,10 @@
     </row>
     <row r="342" spans="1:3">
       <c r="A342" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="B342" t="s">
-        <v>217</v>
+        <v>321</v>
       </c>
       <c r="C342">
         <v>7</v>
@@ -6590,10 +6602,10 @@
     </row>
     <row r="343" spans="1:3">
       <c r="A343" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="B343" t="s">
-        <v>348</v>
+        <v>94</v>
       </c>
       <c r="C343">
         <v>7</v>
@@ -6601,10 +6613,10 @@
     </row>
     <row r="344" spans="1:3">
       <c r="A344" t="s">
-        <v>608</v>
+        <v>397</v>
       </c>
       <c r="B344" t="s">
-        <v>313</v>
+        <v>217</v>
       </c>
       <c r="C344">
         <v>7</v>
@@ -6612,10 +6624,10 @@
     </row>
     <row r="345" spans="1:3">
       <c r="A345" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="B345" t="s">
-        <v>216</v>
+        <v>348</v>
       </c>
       <c r="C345">
         <v>7</v>
@@ -6623,10 +6635,10 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B346" t="s">
-        <v>615</v>
+        <v>313</v>
       </c>
       <c r="C346">
         <v>7</v>
@@ -6634,21 +6646,21 @@
     </row>
     <row r="347" spans="1:3">
       <c r="A347" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B347" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="C347">
         <v>7</v>
       </c>
     </row>
     <row r="348" spans="1:3">
-      <c r="A348" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>403</v>
+      <c r="A348" t="s">
+        <v>616</v>
+      </c>
+      <c r="B348" t="s">
+        <v>615</v>
       </c>
       <c r="C348">
         <v>7</v>
@@ -6656,21 +6668,21 @@
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
-        <v>412</v>
+        <v>381</v>
       </c>
       <c r="B349" t="s">
-        <v>413</v>
+        <v>235</v>
       </c>
       <c r="C349">
         <v>7</v>
       </c>
     </row>
     <row r="350" spans="1:3">
-      <c r="A350" t="s">
-        <v>428</v>
-      </c>
-      <c r="B350" t="s">
-        <v>429</v>
+      <c r="A350" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B350" s="3" t="s">
+        <v>403</v>
       </c>
       <c r="C350">
         <v>7</v>
@@ -6678,10 +6690,10 @@
     </row>
     <row r="351" spans="1:3">
       <c r="A351" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B351" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="C351">
         <v>7</v>
@@ -6689,10 +6701,10 @@
     </row>
     <row r="352" spans="1:3">
       <c r="A352" t="s">
-        <v>620</v>
+        <v>428</v>
       </c>
       <c r="B352" t="s">
-        <v>619</v>
+        <v>429</v>
       </c>
       <c r="C352">
         <v>7</v>
@@ -6700,10 +6712,10 @@
     </row>
     <row r="353" spans="1:3">
       <c r="A353" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
       <c r="B353" t="s">
-        <v>460</v>
+        <v>429</v>
       </c>
       <c r="C353">
         <v>7</v>
@@ -6711,10 +6723,10 @@
     </row>
     <row r="354" spans="1:3">
       <c r="A354" t="s">
-        <v>483</v>
+        <v>620</v>
       </c>
       <c r="B354" t="s">
-        <v>220</v>
+        <v>619</v>
       </c>
       <c r="C354">
         <v>7</v>
@@ -6722,10 +6734,10 @@
     </row>
     <row r="355" spans="1:3">
       <c r="A355" t="s">
-        <v>525</v>
+        <v>459</v>
       </c>
       <c r="B355" t="s">
-        <v>265</v>
+        <v>460</v>
       </c>
       <c r="C355">
         <v>7</v>
@@ -6733,10 +6745,10 @@
     </row>
     <row r="356" spans="1:3">
       <c r="A356" t="s">
-        <v>533</v>
+        <v>483</v>
       </c>
       <c r="B356" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="C356">
         <v>7</v>
@@ -6744,7 +6756,7 @@
     </row>
     <row r="357" spans="1:3">
       <c r="A357" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="B357" t="s">
         <v>265</v>
@@ -6755,7 +6767,7 @@
     </row>
     <row r="358" spans="1:3">
       <c r="A358" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B358" t="s">
         <v>265</v>
@@ -6766,7 +6778,7 @@
     </row>
     <row r="359" spans="1:3">
       <c r="A359" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B359" t="s">
         <v>265</v>
@@ -6777,7 +6789,7 @@
     </row>
     <row r="360" spans="1:3">
       <c r="A360" t="s">
-        <v>554</v>
+        <v>535</v>
       </c>
       <c r="B360" t="s">
         <v>265</v>
@@ -6788,7 +6800,7 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" t="s">
-        <v>562</v>
+        <v>537</v>
       </c>
       <c r="B361" t="s">
         <v>265</v>
@@ -6799,7 +6811,7 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="B362" t="s">
         <v>265</v>
@@ -6810,7 +6822,7 @@
     </row>
     <row r="363" spans="1:3">
       <c r="A363" t="s">
-        <v>609</v>
+        <v>562</v>
       </c>
       <c r="B363" t="s">
         <v>265</v>
@@ -6821,7 +6833,7 @@
     </row>
     <row r="364" spans="1:3">
       <c r="A364" t="s">
-        <v>634</v>
+        <v>563</v>
       </c>
       <c r="B364" t="s">
         <v>265</v>
@@ -6832,10 +6844,10 @@
     </row>
     <row r="365" spans="1:3">
       <c r="A365" t="s">
-        <v>550</v>
+        <v>609</v>
       </c>
       <c r="B365" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="C365">
         <v>7</v>
@@ -6843,51 +6855,51 @@
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
-        <v>536</v>
+        <v>634</v>
       </c>
       <c r="B366" t="s">
         <v>265</v>
       </c>
       <c r="C366">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367" t="s">
-        <v>654</v>
+        <v>740</v>
       </c>
       <c r="B367" t="s">
-        <v>265</v>
+        <v>741</v>
       </c>
       <c r="C367">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="A368" t="s">
-        <v>546</v>
+        <v>742</v>
       </c>
       <c r="B368" t="s">
-        <v>265</v>
+        <v>741</v>
       </c>
       <c r="C368">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="369" spans="1:3">
       <c r="A369" t="s">
-        <v>661</v>
+        <v>550</v>
       </c>
       <c r="B369" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C369">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="370" spans="1:3">
       <c r="A370" t="s">
-        <v>662</v>
+        <v>536</v>
       </c>
       <c r="B370" t="s">
         <v>265</v>
@@ -6898,10 +6910,10 @@
     </row>
     <row r="371" spans="1:3">
       <c r="A371" t="s">
-        <v>617</v>
+        <v>654</v>
       </c>
       <c r="B371" t="s">
-        <v>606</v>
+        <v>265</v>
       </c>
       <c r="C371">
         <v>8</v>
@@ -6909,10 +6921,10 @@
     </row>
     <row r="372" spans="1:3">
       <c r="A372" t="s">
-        <v>611</v>
+        <v>546</v>
       </c>
       <c r="B372" t="s">
-        <v>588</v>
+        <v>265</v>
       </c>
       <c r="C372">
         <v>8</v>
@@ -6920,10 +6932,10 @@
     </row>
     <row r="373" spans="1:3">
       <c r="A373" t="s">
-        <v>485</v>
+        <v>661</v>
       </c>
       <c r="B373" t="s">
-        <v>220</v>
+        <v>265</v>
       </c>
       <c r="C373">
         <v>8</v>
@@ -6931,7 +6943,7 @@
     </row>
     <row r="374" spans="1:3">
       <c r="A374" t="s">
-        <v>605</v>
+        <v>662</v>
       </c>
       <c r="B374" t="s">
         <v>265</v>
@@ -6942,10 +6954,10 @@
     </row>
     <row r="375" spans="1:3">
       <c r="A375" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B375" t="s">
-        <v>367</v>
+        <v>606</v>
       </c>
       <c r="C375">
         <v>8</v>
@@ -6953,10 +6965,10 @@
     </row>
     <row r="376" spans="1:3">
       <c r="A376" t="s">
-        <v>667</v>
+        <v>611</v>
       </c>
       <c r="B376" t="s">
-        <v>547</v>
+        <v>588</v>
       </c>
       <c r="C376">
         <v>8</v>
@@ -6964,10 +6976,10 @@
     </row>
     <row r="377" spans="1:3">
       <c r="A377" t="s">
-        <v>668</v>
+        <v>485</v>
       </c>
       <c r="B377" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="C377">
         <v>8</v>
@@ -6975,10 +6987,10 @@
     </row>
     <row r="378" spans="1:3">
       <c r="A378" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="B378" t="s">
-        <v>492</v>
+        <v>265</v>
       </c>
       <c r="C378">
         <v>8</v>
@@ -6986,10 +6998,10 @@
     </row>
     <row r="379" spans="1:3">
       <c r="A379" t="s">
-        <v>629</v>
+        <v>610</v>
       </c>
       <c r="B379" t="s">
-        <v>449</v>
+        <v>367</v>
       </c>
       <c r="C379">
         <v>8</v>
@@ -6997,10 +7009,10 @@
     </row>
     <row r="380" spans="1:3">
       <c r="A380" t="s">
-        <v>555</v>
+        <v>667</v>
       </c>
       <c r="B380" t="s">
-        <v>376</v>
+        <v>547</v>
       </c>
       <c r="C380">
         <v>8</v>
@@ -7008,10 +7020,10 @@
     </row>
     <row r="381" spans="1:3">
       <c r="A381" t="s">
-        <v>556</v>
+        <v>668</v>
       </c>
       <c r="B381" t="s">
-        <v>557</v>
+        <v>253</v>
       </c>
       <c r="C381">
         <v>8</v>
@@ -7019,32 +7031,32 @@
     </row>
     <row r="382" spans="1:3">
       <c r="A382" t="s">
-        <v>558</v>
+        <v>628</v>
       </c>
       <c r="B382" t="s">
-        <v>333</v>
+        <v>492</v>
       </c>
       <c r="C382">
         <v>8</v>
       </c>
     </row>
     <row r="383" spans="1:3">
-      <c r="A383" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="B383" s="3" t="s">
-        <v>560</v>
+      <c r="A383" t="s">
+        <v>629</v>
+      </c>
+      <c r="B383" t="s">
+        <v>449</v>
       </c>
       <c r="C383">
         <v>8</v>
       </c>
     </row>
     <row r="384" spans="1:3">
-      <c r="A384" s="3" t="s">
-        <v>584</v>
+      <c r="A384" t="s">
+        <v>555</v>
       </c>
       <c r="B384" t="s">
-        <v>585</v>
+        <v>376</v>
       </c>
       <c r="C384">
         <v>8</v>
@@ -7052,10 +7064,10 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" t="s">
-        <v>599</v>
+        <v>556</v>
       </c>
       <c r="B385" t="s">
-        <v>600</v>
+        <v>557</v>
       </c>
       <c r="C385">
         <v>8</v>
@@ -7063,32 +7075,32 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" t="s">
-        <v>603</v>
+        <v>558</v>
       </c>
       <c r="B386" t="s">
-        <v>600</v>
+        <v>333</v>
       </c>
       <c r="C386">
         <v>8</v>
       </c>
     </row>
     <row r="387" spans="1:4">
-      <c r="A387" t="s">
-        <v>601</v>
-      </c>
-      <c r="B387" t="s">
-        <v>600</v>
+      <c r="A387" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B387" s="3" t="s">
+        <v>560</v>
       </c>
       <c r="C387">
         <v>8</v>
       </c>
     </row>
     <row r="388" spans="1:4">
-      <c r="A388" t="s">
-        <v>602</v>
+      <c r="A388" s="3" t="s">
+        <v>584</v>
       </c>
       <c r="B388" t="s">
-        <v>600</v>
+        <v>585</v>
       </c>
       <c r="C388">
         <v>8</v>
@@ -7096,7 +7108,7 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B389" t="s">
         <v>600</v>
@@ -7107,7 +7119,7 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B390" t="s">
         <v>600</v>
@@ -7117,80 +7129,124 @@
       </c>
     </row>
     <row r="391" spans="1:4">
-      <c r="A391" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="B391" s="3" t="s">
-        <v>544</v>
+      <c r="A391" t="s">
+        <v>601</v>
+      </c>
+      <c r="B391" t="s">
+        <v>600</v>
       </c>
       <c r="C391">
-        <v>9</v>
-      </c>
-      <c r="D391" t="s">
-        <v>545</v>
+        <v>8</v>
       </c>
     </row>
     <row r="392" spans="1:4">
-      <c r="A392" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="B392" s="3"/>
+      <c r="A392" t="s">
+        <v>602</v>
+      </c>
+      <c r="B392" t="s">
+        <v>600</v>
+      </c>
       <c r="C392">
-        <v>9</v>
-      </c>
-      <c r="D392" t="s">
-        <v>568</v>
+        <v>8</v>
       </c>
     </row>
     <row r="393" spans="1:4">
-      <c r="A393" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="B393" s="3"/>
+      <c r="A393" t="s">
+        <v>604</v>
+      </c>
+      <c r="B393" t="s">
+        <v>600</v>
+      </c>
       <c r="C393">
-        <v>9</v>
-      </c>
-      <c r="D393" t="s">
-        <v>643</v>
+        <v>8</v>
       </c>
     </row>
     <row r="394" spans="1:4">
-      <c r="A394" s="3" t="s">
-        <v>630</v>
+      <c r="A394" t="s">
+        <v>604</v>
+      </c>
+      <c r="B394" t="s">
+        <v>600</v>
       </c>
       <c r="C394">
-        <v>9</v>
-      </c>
-      <c r="D394" t="s">
-        <v>631</v>
+        <v>8</v>
       </c>
     </row>
     <row r="395" spans="1:4">
       <c r="A395" s="3" t="s">
-        <v>640</v>
+        <v>543</v>
+      </c>
+      <c r="B395" s="3" t="s">
+        <v>544</v>
       </c>
       <c r="C395">
         <v>9</v>
       </c>
       <c r="D395" t="s">
-        <v>641</v>
+        <v>545</v>
       </c>
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="3" t="s">
-        <v>656</v>
-      </c>
+        <v>567</v>
+      </c>
+      <c r="B396" s="3"/>
       <c r="C396">
         <v>9</v>
       </c>
       <c r="D396" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4">
+      <c r="A397" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B397" s="3"/>
+      <c r="C397">
+        <v>9</v>
+      </c>
+      <c r="D397" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4">
+      <c r="A398" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C398">
+        <v>9</v>
+      </c>
+      <c r="D398" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4">
+      <c r="A399" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C399">
+        <v>9</v>
+      </c>
+      <c r="D399" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4">
+      <c r="A400" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C400">
+        <v>9</v>
+      </c>
+      <c r="D400" t="s">
         <v>657</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:D321">
-    <sortCondition ref="C32:C321"/>
-    <sortCondition ref="A32:A321"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:D323">
+    <sortCondition ref="C32:C323"/>
+    <sortCondition ref="A32:A323"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Incorporate currency changes in QUDT
USDollar changed to CCY_US  - substitutions changed
</commit_message>
<xml_diff>
--- a/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
+++ b/RCode_JP/DataFiles4R/SingularAbbrevsTablewQUDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jhp7e\Box Sync\EMLUnits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4578DA84-D3F9-407F-A7B0-8C37FD08D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4FC846-8419-4A8A-A03D-878F3DD7AC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="5625" windowWidth="21600" windowHeight="11295" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
+    <workbookView xWindow="4125" yWindow="1245" windowWidth="21615" windowHeight="11295" xr2:uid="{455CDFE1-8167-4B8E-A1F9-33E0FFDB7CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1211,9 +1211,6 @@
     <t>dollar</t>
   </si>
   <si>
-    <t>USDollar</t>
-  </si>
-  <si>
     <t>micromols</t>
   </si>
   <si>
@@ -1250,9 +1247,6 @@
     <t>1e6dollars</t>
   </si>
   <si>
-    <t>MillionUSD</t>
-  </si>
-  <si>
     <t>centemeter</t>
   </si>
   <si>
@@ -2316,6 +2310,12 @@
   </si>
   <si>
     <t>killo</t>
+  </si>
+  <si>
+    <t>CCY_USD</t>
+  </si>
+  <si>
+    <t>MegaCCY_USD</t>
   </si>
 </sst>
 </file>
@@ -2730,8 +2730,8 @@
   <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B305" sqref="B305"/>
+      <pane ySplit="1" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A384" sqref="A384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2756,10 +2756,10 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1">
       <c r="A2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B3" t="s">
         <v>234</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B4" t="s">
         <v>265</v>
@@ -2789,10 +2789,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2800,10 +2800,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B7" t="s">
         <v>234</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B8" t="s">
         <v>211</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B9" t="s">
         <v>271</v>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2856,10 +2856,10 @@
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B13" t="s">
         <v>333</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B14" t="s">
         <v>247</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B15" t="s">
         <v>341</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B16" t="s">
         <v>272</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B17" t="s">
         <v>246</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B18" t="s">
         <v>236</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="19" spans="1:4" s="4" customFormat="1">
       <c r="A19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B19" t="s">
         <v>355</v>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1">
       <c r="A20" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2970,10 +2970,10 @@
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1">
       <c r="A21" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B21" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="22" spans="1:4" s="4" customFormat="1">
       <c r="A22" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B22" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2994,10 +2994,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B23" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3005,10 +3005,10 @@
     </row>
     <row r="24" spans="1:4" s="4" customFormat="1">
       <c r="A24" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B24" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3017,10 +3017,10 @@
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1">
       <c r="A25" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B25" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3029,10 +3029,10 @@
     </row>
     <row r="26" spans="1:4" s="4" customFormat="1">
       <c r="A26" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B26" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3041,10 +3041,10 @@
     </row>
     <row r="27" spans="1:4" s="4" customFormat="1">
       <c r="A27" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B27" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="28" spans="1:4" s="4" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B28" t="s">
         <v>214</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="29" spans="1:4" s="4" customFormat="1">
       <c r="A29" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B29" t="s">
         <v>214</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1">
       <c r="A30" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B30" t="s">
         <v>281</v>
@@ -3089,10 +3089,10 @@
     </row>
     <row r="31" spans="1:4" s="4" customFormat="1">
       <c r="A31" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B31" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3104,7 +3104,7 @@
         <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3123,10 +3123,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B34" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3134,10 +3134,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B35" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3145,10 +3145,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B36" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B37" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B38" t="s">
         <v>196</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B39" t="s">
         <v>196</v>
@@ -3189,10 +3189,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B40" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B41" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3211,10 +3211,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3222,10 +3222,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3233,10 +3233,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B44" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3244,10 +3244,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B45" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B46" t="s">
         <v>265</v>
@@ -3266,10 +3266,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B48" t="s">
         <v>255</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B49" t="s">
         <v>255</v>
@@ -3299,10 +3299,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B50" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3310,10 +3310,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B51" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B52" t="s">
         <v>234</v>
@@ -3332,10 +3332,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B53" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B54" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3354,10 +3354,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B55" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3365,10 +3365,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B56" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3376,10 +3376,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3387,10 +3387,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B58" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3398,10 +3398,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B59" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3409,10 +3409,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>234</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B62" t="s">
         <v>250</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B63" t="s">
         <v>234</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B64" t="s">
         <v>220</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B65" t="s">
         <v>234</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B66" t="s">
         <v>265</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B67" t="s">
         <v>321</v>
@@ -3497,10 +3497,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B68" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3508,10 +3508,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3519,10 +3519,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -3530,10 +3530,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3541,10 +3541,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>261</v>
@@ -3563,10 +3563,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3577,7 +3577,7 @@
         <v>275</v>
       </c>
       <c r="B75" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -3585,10 +3585,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B76" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -3599,7 +3599,7 @@
         <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -3607,10 +3607,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B78" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C78">
         <v>2</v>
@@ -3618,10 +3618,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B79" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C79">
         <v>2</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B81" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B82" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -3665,10 +3665,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B83" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B84" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3687,10 +3687,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B85" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3698,24 +3698,24 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B86" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B87" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -3756,7 +3756,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B91" t="s">
         <v>267</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B93" t="s">
         <v>267</v>
@@ -3789,10 +3789,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B94" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C94">
         <v>2</v>
@@ -3800,24 +3800,24 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B95" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B96" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C96">
         <v>2</v>
@@ -3825,10 +3825,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B97" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -3839,7 +3839,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B98" t="s">
         <v>341</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B99" t="s">
         <v>234</v>
@@ -3861,7 +3861,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B100" t="s">
         <v>272</v>
@@ -3872,7 +3872,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B101" t="s">
         <v>272</v>
@@ -3883,10 +3883,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B102" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C102">
         <v>2</v>
@@ -3894,7 +3894,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B103" t="s">
         <v>307</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B104" t="s">
         <v>307</v>
@@ -3916,10 +3916,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B105" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -3927,10 +3927,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B106" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C106">
         <v>2</v>
@@ -3938,10 +3938,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B107" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C107">
         <v>2</v>
@@ -3949,10 +3949,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B108" t="s">
-        <v>389</v>
+        <v>744</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -3960,10 +3960,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B109" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C109">
         <v>3</v>
@@ -3971,7 +3971,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B110" t="s">
         <v>356</v>
@@ -3982,10 +3982,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B111" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -4004,10 +4004,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B113" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C113">
         <v>3</v>
@@ -4015,10 +4015,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B114" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B115" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C115">
         <v>3</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B119" t="s">
         <v>213</v>
@@ -4084,7 +4084,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B120" t="s">
         <v>338</v>
@@ -4106,10 +4106,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B122" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C122">
         <v>3</v>
@@ -4120,7 +4120,7 @@
         <v>195</v>
       </c>
       <c r="B123" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C123">
         <v>3</v>
@@ -4150,10 +4150,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B126" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C126">
         <v>3</v>
@@ -4161,7 +4161,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B127" t="s">
         <v>281</v>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B129" t="s">
         <v>281</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B130" t="s">
         <v>281</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B131" t="s">
         <v>281</v>
@@ -4233,10 +4233,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B133" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C133">
         <v>2</v>
@@ -4244,10 +4244,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B134" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C134">
         <v>3</v>
@@ -4255,10 +4255,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B135" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C135">
         <v>3</v>
@@ -4277,10 +4277,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B137" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -4299,10 +4299,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B139" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -4310,21 +4310,21 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B140" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C140">
         <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B141" t="s">
         <v>313</v>
@@ -4346,24 +4346,24 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B143" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C143">
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B144" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C144">
         <v>3</v>
@@ -4371,24 +4371,24 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B145" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C145">
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B146" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C146">
         <v>3</v>
@@ -4451,7 +4451,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B152" t="s">
         <v>259</v>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B156" t="s">
         <v>264</v>
@@ -4517,10 +4517,10 @@
     </row>
     <row r="158" spans="1:4" s="4" customFormat="1">
       <c r="A158" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B158" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C158">
         <v>3</v>
@@ -4529,10 +4529,10 @@
     </row>
     <row r="159" spans="1:4" s="4" customFormat="1">
       <c r="A159" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B159" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C159">
         <v>4</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B160" t="s">
         <v>333</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B162" t="s">
         <v>333</v>
@@ -4580,7 +4580,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B163" t="s">
         <v>333</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B164" t="s">
         <v>348</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B166" t="s">
         <v>261</v>
@@ -4622,12 +4622,12 @@
         <v>3</v>
       </c>
       <c r="D166" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B167" t="s">
         <v>261</v>
@@ -4641,7 +4641,7 @@
         <v>43</v>
       </c>
       <c r="B168" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C168">
         <v>3</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B169" t="s">
         <v>338</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B173" t="s">
         <v>243</v>
@@ -4729,10 +4729,10 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B176" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C176">
         <v>3</v>
@@ -4751,10 +4751,10 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B178" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C178">
         <v>3</v>
@@ -4773,10 +4773,10 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B180" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C180">
         <v>3</v>
@@ -4787,10 +4787,10 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B181" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C181">
         <v>3</v>
@@ -4798,10 +4798,10 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B182" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C182">
         <v>3</v>
@@ -4834,7 +4834,7 @@
         <v>46</v>
       </c>
       <c r="B185" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C185">
         <v>3</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B186" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C186">
         <v>3</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B187" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C187">
         <v>3</v>
@@ -4864,10 +4864,10 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B188" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C188">
         <v>3</v>
@@ -4875,10 +4875,10 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B189" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C189">
         <v>3</v>
@@ -5007,10 +5007,10 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B201" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C201">
         <v>3</v>
@@ -5018,7 +5018,7 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B202" t="s">
         <v>196</v>
@@ -5073,7 +5073,7 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B207" t="s">
         <v>226</v>
@@ -5167,10 +5167,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B215" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C215">
         <v>5</v>
@@ -5178,10 +5178,10 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B216" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C216">
         <v>5</v>
@@ -5200,10 +5200,10 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B218" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C218">
         <v>5</v>
@@ -5211,10 +5211,10 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B219" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C219">
         <v>5</v>
@@ -5222,10 +5222,10 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B220" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C220">
         <v>5</v>
@@ -5233,10 +5233,10 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B221" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C221">
         <v>5</v>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B223" t="s">
         <v>244</v>
@@ -5280,10 +5280,10 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B225" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C225">
         <v>5</v>
@@ -5291,10 +5291,10 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B226" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C226">
         <v>5</v>
@@ -5324,7 +5324,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B229" t="s">
         <v>214</v>
@@ -5338,10 +5338,10 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B230" t="s">
-        <v>376</v>
+        <v>743</v>
       </c>
       <c r="C230">
         <v>5</v>
@@ -5349,10 +5349,10 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B231" t="s">
-        <v>376</v>
+        <v>743</v>
       </c>
       <c r="C231">
         <v>5</v>
@@ -5363,7 +5363,7 @@
         <v>375</v>
       </c>
       <c r="B232" t="s">
-        <v>376</v>
+        <v>743</v>
       </c>
       <c r="C232">
         <v>5</v>
@@ -5382,10 +5382,10 @@
     </row>
     <row r="234" spans="1:4" s="4" customFormat="1">
       <c r="A234" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B234" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C234">
         <v>5</v>
@@ -5393,7 +5393,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B235" t="s">
         <v>255</v>
@@ -5407,7 +5407,7 @@
         <v>22</v>
       </c>
       <c r="B236" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C236">
         <v>5</v>
@@ -5415,7 +5415,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B237" t="s">
         <v>255</v>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B238" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C238">
         <v>5</v>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B247" t="s">
         <v>217</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B250" t="s">
         <v>248</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B253" t="s">
         <v>94</v>
@@ -5624,7 +5624,7 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B256" t="s">
         <v>220</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B266" t="s">
         <v>234</v>
@@ -5781,10 +5781,10 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B270" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C270">
         <v>5</v>
@@ -5847,10 +5847,10 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B276" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C276">
         <v>5</v>
@@ -5927,7 +5927,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B283" t="s">
         <v>244</v>
@@ -5941,10 +5941,10 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B284" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C284">
         <v>6</v>
@@ -5952,10 +5952,10 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B285" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C285">
         <v>6</v>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B286" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C286">
         <v>6</v>
@@ -5974,10 +5974,10 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B287" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C287">
         <v>6</v>
@@ -5985,10 +5985,10 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B288" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C288">
         <v>6</v>
@@ -5996,10 +5996,10 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B289" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C289">
         <v>6</v>
@@ -6007,10 +6007,10 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B290" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C290">
         <v>6</v>
@@ -6018,10 +6018,10 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B291" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C291">
         <v>6</v>
@@ -6029,10 +6029,10 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B292" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C292">
         <v>6</v>
@@ -6040,10 +6040,10 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B293" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C293">
         <v>6</v>
@@ -6076,10 +6076,10 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B296" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C296">
         <v>6</v>
@@ -6087,10 +6087,10 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B297" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C297">
         <v>6</v>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B298" t="s">
         <v>370</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B301" t="s">
         <v>296</v>
@@ -6142,7 +6142,7 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B302" t="s">
         <v>296</v>
@@ -6161,7 +6161,7 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B304" t="s">
         <v>298</v>
@@ -6194,7 +6194,7 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B307" t="s">
         <v>344</v>
@@ -6205,7 +6205,7 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B308" t="s">
         <v>344</v>
@@ -6227,7 +6227,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B310" t="s">
         <v>301</v>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B312" t="s">
         <v>301</v>
@@ -6258,12 +6258,12 @@
         <v>6</v>
       </c>
       <c r="D312" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="313" spans="1:4">
       <c r="A313" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B313" t="s">
         <v>301</v>
@@ -6272,7 +6272,7 @@
         <v>6</v>
       </c>
       <c r="D313" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6299,10 +6299,10 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B316" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C316">
         <v>6</v>
@@ -6310,10 +6310,10 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B317" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C317">
         <v>6</v>
@@ -6393,10 +6393,10 @@
     </row>
     <row r="324" spans="1:3">
       <c r="A324" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B324" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C324">
         <v>6</v>
@@ -6404,10 +6404,10 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B325" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C325">
         <v>6</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="333" spans="1:3">
       <c r="A333" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B333" t="s">
         <v>355</v>
@@ -6514,10 +6514,10 @@
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B335" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C335">
         <v>6</v>
@@ -6525,10 +6525,10 @@
     </row>
     <row r="336" spans="1:3">
       <c r="A336" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B336" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C336">
         <v>6</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="338" spans="1:3">
       <c r="A338" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B338" t="s">
         <v>307</v>
@@ -6569,7 +6569,7 @@
     </row>
     <row r="340" spans="1:3">
       <c r="A340" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B340" t="s">
         <v>294</v>
@@ -6580,10 +6580,10 @@
     </row>
     <row r="341" spans="1:3">
       <c r="A341" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B341" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C341">
         <v>7</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="342" spans="1:3">
       <c r="A342" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B342" t="s">
         <v>321</v>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="343" spans="1:3">
       <c r="A343" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B343" t="s">
         <v>94</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="344" spans="1:3">
       <c r="A344" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B344" t="s">
         <v>217</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="345" spans="1:3">
       <c r="A345" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B345" t="s">
         <v>348</v>
@@ -6635,7 +6635,7 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B346" t="s">
         <v>313</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="347" spans="1:3">
       <c r="A347" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B347" t="s">
         <v>216</v>
@@ -6657,10 +6657,10 @@
     </row>
     <row r="348" spans="1:3">
       <c r="A348" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B348" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C348">
         <v>7</v>
@@ -6668,7 +6668,7 @@
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B349" t="s">
         <v>235</v>
@@ -6679,10 +6679,10 @@
     </row>
     <row r="350" spans="1:3">
       <c r="A350" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C350">
         <v>7</v>
@@ -6690,10 +6690,10 @@
     </row>
     <row r="351" spans="1:3">
       <c r="A351" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B351" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C351">
         <v>7</v>
@@ -6701,10 +6701,10 @@
     </row>
     <row r="352" spans="1:3">
       <c r="A352" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B352" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C352">
         <v>7</v>
@@ -6712,10 +6712,10 @@
     </row>
     <row r="353" spans="1:3">
       <c r="A353" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B353" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C353">
         <v>7</v>
@@ -6723,10 +6723,10 @@
     </row>
     <row r="354" spans="1:3">
       <c r="A354" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B354" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C354">
         <v>7</v>
@@ -6734,10 +6734,10 @@
     </row>
     <row r="355" spans="1:3">
       <c r="A355" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B355" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C355">
         <v>7</v>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="356" spans="1:3">
       <c r="A356" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B356" t="s">
         <v>220</v>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="357" spans="1:3">
       <c r="A357" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B357" t="s">
         <v>265</v>
@@ -6767,7 +6767,7 @@
     </row>
     <row r="358" spans="1:3">
       <c r="A358" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B358" t="s">
         <v>265</v>
@@ -6778,7 +6778,7 @@
     </row>
     <row r="359" spans="1:3">
       <c r="A359" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B359" t="s">
         <v>265</v>
@@ -6789,7 +6789,7 @@
     </row>
     <row r="360" spans="1:3">
       <c r="A360" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B360" t="s">
         <v>265</v>
@@ -6800,7 +6800,7 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B361" t="s">
         <v>265</v>
@@ -6811,7 +6811,7 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B362" t="s">
         <v>265</v>
@@ -6822,7 +6822,7 @@
     </row>
     <row r="363" spans="1:3">
       <c r="A363" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B363" t="s">
         <v>265</v>
@@ -6833,7 +6833,7 @@
     </row>
     <row r="364" spans="1:3">
       <c r="A364" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B364" t="s">
         <v>265</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="365" spans="1:3">
       <c r="A365" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B365" t="s">
         <v>265</v>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B366" t="s">
         <v>265</v>
@@ -6866,10 +6866,10 @@
     </row>
     <row r="367" spans="1:3">
       <c r="A367" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B367" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C367">
         <v>7</v>
@@ -6877,10 +6877,10 @@
     </row>
     <row r="368" spans="1:3">
       <c r="A368" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B368" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C368">
         <v>7</v>
@@ -6888,7 +6888,7 @@
     </row>
     <row r="369" spans="1:3">
       <c r="A369" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B369" t="s">
         <v>250</v>
@@ -6899,7 +6899,7 @@
     </row>
     <row r="370" spans="1:3">
       <c r="A370" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B370" t="s">
         <v>265</v>
@@ -6910,7 +6910,7 @@
     </row>
     <row r="371" spans="1:3">
       <c r="A371" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B371" t="s">
         <v>265</v>
@@ -6921,7 +6921,7 @@
     </row>
     <row r="372" spans="1:3">
       <c r="A372" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B372" t="s">
         <v>265</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="373" spans="1:3">
       <c r="A373" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B373" t="s">
         <v>265</v>
@@ -6943,7 +6943,7 @@
     </row>
     <row r="374" spans="1:3">
       <c r="A374" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B374" t="s">
         <v>265</v>
@@ -6954,10 +6954,10 @@
     </row>
     <row r="375" spans="1:3">
       <c r="A375" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B375" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C375">
         <v>8</v>
@@ -6965,10 +6965,10 @@
     </row>
     <row r="376" spans="1:3">
       <c r="A376" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B376" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C376">
         <v>8</v>
@@ -6976,7 +6976,7 @@
     </row>
     <row r="377" spans="1:3">
       <c r="A377" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B377" t="s">
         <v>220</v>
@@ -6987,7 +6987,7 @@
     </row>
     <row r="378" spans="1:3">
       <c r="A378" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B378" t="s">
         <v>265</v>
@@ -6998,7 +6998,7 @@
     </row>
     <row r="379" spans="1:3">
       <c r="A379" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B379" t="s">
         <v>367</v>
@@ -7009,10 +7009,10 @@
     </row>
     <row r="380" spans="1:3">
       <c r="A380" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B380" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C380">
         <v>8</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="381" spans="1:3">
       <c r="A381" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B381" t="s">
         <v>253</v>
@@ -7031,10 +7031,10 @@
     </row>
     <row r="382" spans="1:3">
       <c r="A382" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B382" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C382">
         <v>8</v>
@@ -7042,10 +7042,10 @@
     </row>
     <row r="383" spans="1:3">
       <c r="A383" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B383" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C383">
         <v>8</v>
@@ -7053,10 +7053,10 @@
     </row>
     <row r="384" spans="1:3">
       <c r="A384" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B384" t="s">
-        <v>376</v>
+        <v>743</v>
       </c>
       <c r="C384">
         <v>8</v>
@@ -7064,10 +7064,10 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B385" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C385">
         <v>8</v>
@@ -7075,7 +7075,7 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B386" t="s">
         <v>333</v>
@@ -7086,10 +7086,10 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C387">
         <v>8</v>
@@ -7097,10 +7097,10 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B388" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C388">
         <v>8</v>
@@ -7108,10 +7108,10 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B389" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C389">
         <v>8</v>
@@ -7119,10 +7119,10 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B390" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C390">
         <v>8</v>
@@ -7130,10 +7130,10 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B391" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C391">
         <v>8</v>
@@ -7141,10 +7141,10 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B392" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C392">
         <v>8</v>
@@ -7152,10 +7152,10 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B393" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C393">
         <v>8</v>
@@ -7163,10 +7163,10 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B394" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C394">
         <v>8</v>
@@ -7174,73 +7174,73 @@
     </row>
     <row r="395" spans="1:4">
       <c r="A395" s="3" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C395">
         <v>9</v>
       </c>
       <c r="D395" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B396" s="3"/>
       <c r="C396">
         <v>9</v>
       </c>
       <c r="D396" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="3" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B397" s="3"/>
       <c r="C397">
         <v>9</v>
       </c>
       <c r="D397" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="3" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C398">
         <v>9</v>
       </c>
       <c r="D398" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C399">
         <v>9</v>
       </c>
       <c r="D399" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="400" spans="1:4">
       <c r="A400" s="3" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C400">
         <v>9</v>
       </c>
       <c r="D400" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>